<commit_message>
Start implementing the hough transform
</commit_message>
<xml_diff>
--- a/reports/report_tangential_02.xlsx
+++ b/reports/report_tangential_02.xlsx
@@ -882,11 +882,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="9968929"/>
-        <c:axId val="2580845"/>
+        <c:axId val="83691200"/>
+        <c:axId val="45005523"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="9968929"/>
+        <c:axId val="83691200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -968,12 +968,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2580845"/>
+        <c:crossAx val="45005523"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2580845"/>
+        <c:axId val="45005523"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1055,7 +1055,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9968929"/>
+        <c:crossAx val="83691200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1554,11 +1554,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="79577452"/>
-        <c:axId val="51448675"/>
+        <c:axId val="74617761"/>
+        <c:axId val="88789684"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79577452"/>
+        <c:axId val="74617761"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1640,12 +1640,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51448675"/>
+        <c:crossAx val="88789684"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51448675"/>
+        <c:axId val="88789684"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1727,7 +1727,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79577452"/>
+        <c:crossAx val="74617761"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2226,11 +2226,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="84912462"/>
-        <c:axId val="41769486"/>
+        <c:axId val="65560094"/>
+        <c:axId val="2012866"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84912462"/>
+        <c:axId val="65560094"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2312,12 +2312,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41769486"/>
+        <c:crossAx val="2012866"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="41769486"/>
+        <c:axId val="2012866"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2399,7 +2399,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84912462"/>
+        <c:crossAx val="65560094"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2898,11 +2898,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="38963341"/>
-        <c:axId val="52115158"/>
+        <c:axId val="15814883"/>
+        <c:axId val="99168342"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="38963341"/>
+        <c:axId val="15814883"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2984,12 +2984,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52115158"/>
+        <c:crossAx val="99168342"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52115158"/>
+        <c:axId val="99168342"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3071,7 +3071,682 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38963341"/>
+        <c:crossAx val="15814883"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Relative fitting error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet!$G$2:$G$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>0.254152329921264</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.283731313574599</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.255099506011595</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.262673043430365</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.273763801805294</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.272902262960878</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.242106913921383</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.271420571346255</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.277937693285835</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.266711330943551</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.245086857971084</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.236611097819895</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.228228208735704</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.250336917134442</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.247307977022419</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.222956655801872</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.239679012754877</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.236268821293387</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.234161070303585</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.218172863159004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.224735883210392</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.212197152516801</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.197178208269343</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.185696103895107</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.194389864309685</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.163789550764215</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.156865937014098</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.171918065687233</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.170537043382735</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.16292626117652</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.167306672427507</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.15554150906049</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.149946189616682</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.145521132270116</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.153045899312528</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.154226325114427</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.164566412963384</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.168664495990638</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.171567046228351</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.187287236640964</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.184512765010811</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.194335757336477</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.191216322253823</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.191415747804259</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.174214092390487</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.179141390292382</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.179663531486811</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.174319390572369</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.175908792027389</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.180113057543175</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.17177698211152</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.168482314416982</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.174447894742866</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.169886341311027</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.170971957293135</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.168409023020595</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.168825347559584</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.170019735468351</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.158937367542161</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.173636771971415</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.163177277002349</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.165234088902838</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.151325426056621</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.170079443928248</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.167285427945631</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.156823906166187</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet!$L$2:$L$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>3.54987675595424E-007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.72682449530291E-007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.77230313231761E-007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.74011431774948E-007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0194720381037E-007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.48996974300956E-007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7245631237875E-007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.76539897696395E-007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.84152060209206E-007</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.80468150589324E-007</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.71896709527765E-007</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.48507235137188E-007</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.69966933183989E-007</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.58952865599309E-007</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.47725903061085E-007</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.30210701987966E-007</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.38204185358457E-007</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.41279522264548E-007</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.28279899519403E-007</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.15951393035061E-007</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.20203959017912E-007</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.01388186396568E-007</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.89913575234253E-008</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.48478575971147E-008</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.75711390597313E-008</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.80986118807266E-008</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7.27626388577227E-008</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.42153375843499E-008</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.61797727410179E-008</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.81887569656947E-007</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7.49838890928078E-008</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.52655561115033E-008</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.25624317689833E-008</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.94480609527385E-008</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.59238555331662E-008</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.12986570577216E-007</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.18098711648997E-007</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.07905826210891E-006</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9.75209151878078E-008</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.53577471053882E-007</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.60721763240212E-007</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.87602237563336E-007</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5.03779757534036E-007</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.02738374710345E-006</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.01482393098271E-007</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.55839594802374E-007</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6.68248365642905E-007</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>8.35736787846614E-007</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>6.94208097740562E-007</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5.94871845966133E-007</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8.68648349665587E-007</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>6.60603201006936E-007</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4.72488953293918E-007</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.99655414938434E-007</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4.57995929990185E-007</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>8.32888845412862E-007</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>7.03594517572335E-007</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>7.09844130799086E-007</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6.94247582030258E-007</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>9.24562112853701E-007</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5.85661313662649E-007</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>9.82727200247819E-007</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.3916633847961E-006</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.91435024579975E-007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="58122834"/>
+        <c:axId val="49554865"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="58122834"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Relative fitting error</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="49554865"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="49554865"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Curvature</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="58122834"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3113,15 +3788,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>141120</xdr:colOff>
+      <xdr:colOff>141480</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>179280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241920</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>11880</xdr:rowOff>
+      <xdr:rowOff>11520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3129,8 +3804,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12621240" y="179280"/>
-        <a:ext cx="5758920" cy="3240000"/>
+        <a:off x="14755680" y="179280"/>
+        <a:ext cx="5758560" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3143,15 +3818,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>910440</xdr:colOff>
+      <xdr:colOff>910800</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>25200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>68760</xdr:colOff>
+      <xdr:colOff>68400</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
+      <xdr:rowOff>47520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3159,8 +3834,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12447720" y="3810960"/>
-        <a:ext cx="5758920" cy="3239640"/>
+        <a:off x="14582160" y="3810960"/>
+        <a:ext cx="5758560" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3173,15 +3848,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>25920</xdr:colOff>
+      <xdr:colOff>26280</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>115920</xdr:rowOff>
+      <xdr:rowOff>116280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>127080</xdr:colOff>
+      <xdr:colOff>126720</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>135000</xdr:rowOff>
+      <xdr:rowOff>134640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3189,8 +3864,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12506040" y="7307640"/>
-        <a:ext cx="5758920" cy="2857680"/>
+        <a:off x="14640480" y="7308000"/>
+        <a:ext cx="5758560" cy="2856960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3203,15 +3878,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>471960</xdr:colOff>
+      <xdr:colOff>472320</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>7200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>570240</xdr:colOff>
+      <xdr:colOff>569880</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3219,12 +3894,42 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12952080" y="10226880"/>
-        <a:ext cx="5756040" cy="2859480"/>
+        <a:off x="15086520" y="10226880"/>
+        <a:ext cx="5755680" cy="2859120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>443520</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>153720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>541080</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>154800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="15057720" y="13405320"/>
+        <a:ext cx="5755680" cy="2858760"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3240,14 +3945,20 @@
   </sheetPr>
   <dimension ref="A1:L65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q73" activeCellId="0" sqref="Q73"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B67" activeCellId="0" sqref="B1:B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7004048582996"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.417004048583"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7246963562753"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.4898785425101"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Average over grid cells
</commit_message>
<xml_diff>
--- a/reports/report_tangential_02.xlsx
+++ b/reports/report_tangential_02.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t xml:space="preserve">File</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">Fitting error total</t>
   </si>
   <si>
+    <t xml:space="preserve">Abs Radius diff</t>
+  </si>
+  <si>
     <t xml:space="preserve">Relative fitting error</t>
   </si>
   <si>
@@ -53,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">Distance from cam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Score</t>
   </si>
   <si>
     <t xml:space="preserve">res/tangential2//LargeSphere_tangential_02.000005.obj</t>
@@ -260,7 +266,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -282,6 +288,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -343,8 +357,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -434,7 +452,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet!$G$1</c:f>
+              <c:f>Sheet!$H$1:$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -468,7 +486,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet!$K$2:$K$67</c:f>
+              <c:f>Sheet!$M$2:$M$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="66"/>
@@ -675,7 +693,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet!$G$2:$G$67</c:f>
+              <c:f>Sheet!$H$2:$H$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="66"/>
@@ -882,11 +900,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="83691200"/>
-        <c:axId val="45005523"/>
+        <c:axId val="43906746"/>
+        <c:axId val="24873608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83691200"/>
+        <c:axId val="43906746"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -968,12 +986,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45005523"/>
+        <c:crossAx val="24873608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45005523"/>
+        <c:axId val="24873608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1055,7 +1073,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83691200"/>
+        <c:crossAx val="43906746"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1106,7 +1124,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet!$I$1</c:f>
+              <c:f>Sheet!$J$1:$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1140,7 +1158,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet!$K$2:$K$67</c:f>
+              <c:f>Sheet!$M$2:$M$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="66"/>
@@ -1347,7 +1365,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet!$I$2:$I$67</c:f>
+              <c:f>Sheet!$J$2:$J$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="66"/>
@@ -1554,11 +1572,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="74617761"/>
-        <c:axId val="88789684"/>
+        <c:axId val="18530387"/>
+        <c:axId val="97196380"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74617761"/>
+        <c:axId val="18530387"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1640,12 +1658,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88789684"/>
+        <c:crossAx val="97196380"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88789684"/>
+        <c:axId val="97196380"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1727,7 +1745,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74617761"/>
+        <c:crossAx val="18530387"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1778,7 +1796,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet!$J$1</c:f>
+              <c:f>Sheet!$K$1:$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1812,218 +1830,218 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
+              <c:f>Sheet!$M$2:$M$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>-915.633833118999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-913.514787864424</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-911.219665735461</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-904.500916807186</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-903.488616612666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-900.91104810545</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-898.928604942916</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-884.4081303076</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-862.41524984676</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-835.517463070681</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-810.968114001913</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-790.779455100395</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-782.004415146655</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-780.755162674451</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-778.636828530828</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-778.495824114239</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-777.416923436149</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-776.152222237845</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-775.472479847163</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-771.407643293807</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-756.174487389124</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-721.702547139754</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-628.115714441663</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-576.273584945456</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-528.184282586059</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-443.857237441114</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-397.503525883761</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-333.981925008314</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-255.402412665557</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-178.722012234352</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-113.076603811607</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-56.1081751651907</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-7.23067478259313</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44.0173311043849</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>99.2120862986552</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>209.798452996868</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>257.242977178053</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>296.141174817834</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>329.558744579851</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>361.848998790195</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>403.453190497187</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>450.876913976468</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>499.187596301615</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>595.988700198403</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>630.97002109498</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>656.043656990909</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>678.164186826258</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>680.940468290473</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>699.067946539061</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>717.965380590367</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>736.930966986826</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>741.561155526141</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>758.400131105185</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>762.644604057758</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>781.9999117313</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>785.419705175335</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>804.093801721934</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>809.357784286451</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>824.548795750479</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>825.256143537636</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>834.92656881569</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>837.801547813215</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>838.899276955448</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>843.423958654543</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>845.123879794779</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>846.008194632081</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Sheet!$K$2:$K$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="66"/>
                 <c:pt idx="0">
-                  <c:v>-915.633833118999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-913.514787864424</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-911.219665735461</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-904.500916807186</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-903.488616612666</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-900.91104810545</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-898.928604942916</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-884.4081303076</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-862.41524984676</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-835.517463070681</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-810.968114001913</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-790.779455100395</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-782.004415146655</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-780.755162674451</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-778.636828530828</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-778.495824114239</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-777.416923436149</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-776.152222237845</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-775.472479847163</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-771.407643293807</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-756.174487389124</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-721.702547139754</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-628.115714441663</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-576.273584945456</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-528.184282586059</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-443.857237441114</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>-397.503525883761</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-333.981925008314</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>-255.402412665557</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>-178.722012234352</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>-113.076603811607</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>-56.1081751651907</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>-7.23067478259313</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>44.0173311043849</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>99.2120862986552</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>209.798452996868</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>257.242977178053</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>296.141174817834</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>329.558744579851</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>361.848998790195</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>403.453190497187</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>450.876913976468</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>499.187596301615</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>595.988700198403</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>630.97002109498</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>656.043656990909</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>678.164186826258</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>680.940468290473</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>699.067946539061</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>717.965380590367</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>736.930966986826</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>741.561155526141</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>758.400131105185</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>762.644604057758</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>781.9999117313</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>785.419705175335</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>804.093801721934</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>809.357784286451</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>824.548795750479</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>825.256143537636</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>834.92656881569</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>837.801547813215</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>838.899276955448</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>843.423958654543</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>845.123879794779</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>846.008194632081</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet!$J$2:$J$67</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="66"/>
-                <c:pt idx="0">
                   <c:v>0.000916933166062979</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -2226,11 +2244,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="65560094"/>
-        <c:axId val="2012866"/>
+        <c:axId val="81503115"/>
+        <c:axId val="72011381"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65560094"/>
+        <c:axId val="81503115"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2312,12 +2330,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2012866"/>
+        <c:crossAx val="72011381"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2012866"/>
+        <c:axId val="72011381"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2399,7 +2417,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65560094"/>
+        <c:crossAx val="81503115"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2450,11 +2468,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet!$L$1</c:f>
+              <c:f>Sheet!$N$1:$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>Score</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2484,7 +2502,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet!$K$2:$K$67</c:f>
+              <c:f>Sheet!$M$2:$M$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="66"/>
@@ -2691,218 +2709,218 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet!$L$2:$L$67</c:f>
+              <c:f>Sheet!$N$2:$N$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="66"/>
                 <c:pt idx="0">
-                  <c:v>3.54987675595424E-007</c:v>
+                  <c:v>11.7074925002381</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.72682449530291E-007</c:v>
+                  <c:v>9.6369163711924</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.77230313231761E-007</c:v>
+                  <c:v>10.9344096652151</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.74011431774948E-007</c:v>
+                  <c:v>9.23845059877731</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0194720381037E-007</c:v>
+                  <c:v>6.13005052140059</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>9.2883245668524</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.48996974300956E-007</c:v>
+                  <c:v>5.77696864936108</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7245631237875E-007</c:v>
+                  <c:v>10.3039520894631</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.76539897696395E-007</c:v>
+                  <c:v>7.36701414693012</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.84152060209206E-007</c:v>
+                  <c:v>6.49232124699877</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.80468150589324E-007</c:v>
+                  <c:v>7.95720133509238</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.71896709527765E-007</c:v>
+                  <c:v>8.23306855818543</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.48507235137188E-007</c:v>
+                  <c:v>6.74334483962026</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.69966933183989E-007</c:v>
+                  <c:v>28.426137450154</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.58952865599309E-007</c:v>
+                  <c:v>9.82208355554416</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.47725903061085E-007</c:v>
+                  <c:v>5.98294881292658</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.30210701987966E-007</c:v>
+                  <c:v>6.36439826236551</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.38204185358457E-007</c:v>
+                  <c:v>5.51165543054635</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.41279522264548E-007</c:v>
+                  <c:v>7.26817344170837</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.28279899519403E-007</c:v>
+                  <c:v>6.39494051636824</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.15951393035061E-007</c:v>
+                  <c:v>6.10585254130293</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.20203959017912E-007</c:v>
+                  <c:v>4.84882084554495</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.01388186396568E-007</c:v>
+                  <c:v>4.6522940989545</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.89913575234253E-008</c:v>
+                  <c:v>5.36279060179313</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.48478575971147E-008</c:v>
+                  <c:v>5.31912977666709</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.75711390597313E-008</c:v>
+                  <c:v>4.53858985225132</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5.80986118807266E-008</c:v>
+                  <c:v>6.88053895196686</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.27626388577227E-008</c:v>
+                  <c:v>7.42948315782078</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5.42153375843499E-008</c:v>
+                  <c:v>5.07901073040449</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5.61797727410179E-008</c:v>
+                  <c:v>3.73042702405506</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.81887569656947E-007</c:v>
+                  <c:v>7.38839540833304</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7.49838890928078E-008</c:v>
+                  <c:v>5.77360148665784</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.52655561115033E-008</c:v>
+                  <c:v>4.77553526731736</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.25624317689833E-008</c:v>
+                  <c:v>5.2129257696228</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.94480609527385E-008</c:v>
+                  <c:v>14.4648030018106</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.59238555331662E-008</c:v>
+                  <c:v>4.60333014734643</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.12986570577216E-007</c:v>
+                  <c:v>5.45138653560424</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.18098711648997E-007</c:v>
+                  <c:v>5.11318449819013</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.07905826210891E-006</c:v>
+                  <c:v>9.06218002994456</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>9.75209151878078E-008</c:v>
+                  <c:v>8.08067012367249</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.53577471053882E-007</c:v>
+                  <c:v>5.40406853514669</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3.60721763240212E-007</c:v>
+                  <c:v>5.32717563007823</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.87602237563336E-007</c:v>
+                  <c:v>6.01637766168512</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>5.03779757534036E-007</c:v>
+                  <c:v>5.42220436604053</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.02738374710345E-006</c:v>
+                  <c:v>5.06783066641163</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4.01482393098271E-007</c:v>
+                  <c:v>5.84387040638457</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4.55839594802374E-007</c:v>
+                  <c:v>6.7563207761349</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>6.68248365642905E-007</c:v>
+                  <c:v>5.9631636395895</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>8.35736787846614E-007</c:v>
+                  <c:v>7.14037677499423</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>6.94208097740562E-007</c:v>
+                  <c:v>5.38547246699794</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>5.94871845966133E-007</c:v>
+                  <c:v>6.61156570202086</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>8.68648349665587E-007</c:v>
+                  <c:v>6.43992794989476</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>6.60603201006936E-007</c:v>
+                  <c:v>5.30407550143819</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4.72488953293918E-007</c:v>
+                  <c:v>4.76620088223653</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>4.99655414938434E-007</c:v>
+                  <c:v>5.31858260123214</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>4.57995929990185E-007</c:v>
+                  <c:v>4.42190537118259</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>8.32888845412862E-007</c:v>
+                  <c:v>5.7681576052667</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v/>
+                  <c:v>5.66035070862931</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>7.03594517572335E-007</c:v>
+                  <c:v>4.77552071710906</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>7.09844130799086E-007</c:v>
+                  <c:v>4.79805431996423</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>6.94247582030258E-007</c:v>
+                  <c:v>4.08697241434145</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>9.24562112853701E-007</c:v>
+                  <c:v>4.95548823275513</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>5.85661313662649E-007</c:v>
+                  <c:v>4.46802347029649</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>9.82727200247819E-007</c:v>
+                  <c:v>4.75493384700057</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.3916633847961E-006</c:v>
+                  <c:v>5.11245986555183</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>6.91435024579975E-007</c:v>
+                  <c:v>5.03077167788965</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="15814883"/>
-        <c:axId val="99168342"/>
+        <c:axId val="32149877"/>
+        <c:axId val="7066783"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="15814883"/>
+        <c:axId val="32149877"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2984,12 +3002,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99168342"/>
+        <c:crossAx val="7066783"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99168342"/>
+        <c:axId val="7066783"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3071,7 +3089,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15814883"/>
+        <c:crossAx val="32149877"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3122,7 +3140,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet!$G$1</c:f>
+              <c:f>Sheet!$H$1:$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3159,7 +3177,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet!$G$2:$G$67</c:f>
+              <c:f>Sheet!$H$2:$H$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="66"/>
@@ -3366,218 +3384,218 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet!$L$2:$L$67</c:f>
+              <c:f>Sheet!$N$2:$N$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="66"/>
                 <c:pt idx="0">
-                  <c:v>3.54987675595424E-007</c:v>
+                  <c:v>11.7074925002381</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.72682449530291E-007</c:v>
+                  <c:v>9.6369163711924</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.77230313231761E-007</c:v>
+                  <c:v>10.9344096652151</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.74011431774948E-007</c:v>
+                  <c:v>9.23845059877731</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0194720381037E-007</c:v>
+                  <c:v>6.13005052140059</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>9.2883245668524</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.48996974300956E-007</c:v>
+                  <c:v>5.77696864936108</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7245631237875E-007</c:v>
+                  <c:v>10.3039520894631</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.76539897696395E-007</c:v>
+                  <c:v>7.36701414693012</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.84152060209206E-007</c:v>
+                  <c:v>6.49232124699877</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.80468150589324E-007</c:v>
+                  <c:v>7.95720133509238</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.71896709527765E-007</c:v>
+                  <c:v>8.23306855818543</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.48507235137188E-007</c:v>
+                  <c:v>6.74334483962026</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.69966933183989E-007</c:v>
+                  <c:v>28.426137450154</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.58952865599309E-007</c:v>
+                  <c:v>9.82208355554416</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.47725903061085E-007</c:v>
+                  <c:v>5.98294881292658</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.30210701987966E-007</c:v>
+                  <c:v>6.36439826236551</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.38204185358457E-007</c:v>
+                  <c:v>5.51165543054635</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.41279522264548E-007</c:v>
+                  <c:v>7.26817344170837</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.28279899519403E-007</c:v>
+                  <c:v>6.39494051636824</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.15951393035061E-007</c:v>
+                  <c:v>6.10585254130293</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.20203959017912E-007</c:v>
+                  <c:v>4.84882084554495</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.01388186396568E-007</c:v>
+                  <c:v>4.6522940989545</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.89913575234253E-008</c:v>
+                  <c:v>5.36279060179313</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.48478575971147E-008</c:v>
+                  <c:v>5.31912977666709</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.75711390597313E-008</c:v>
+                  <c:v>4.53858985225132</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5.80986118807266E-008</c:v>
+                  <c:v>6.88053895196686</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.27626388577227E-008</c:v>
+                  <c:v>7.42948315782078</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5.42153375843499E-008</c:v>
+                  <c:v>5.07901073040449</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5.61797727410179E-008</c:v>
+                  <c:v>3.73042702405506</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.81887569656947E-007</c:v>
+                  <c:v>7.38839540833304</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7.49838890928078E-008</c:v>
+                  <c:v>5.77360148665784</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.52655561115033E-008</c:v>
+                  <c:v>4.77553526731736</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.25624317689833E-008</c:v>
+                  <c:v>5.2129257696228</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.94480609527385E-008</c:v>
+                  <c:v>14.4648030018106</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.59238555331662E-008</c:v>
+                  <c:v>4.60333014734643</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.12986570577216E-007</c:v>
+                  <c:v>5.45138653560424</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.18098711648997E-007</c:v>
+                  <c:v>5.11318449819013</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.07905826210891E-006</c:v>
+                  <c:v>9.06218002994456</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>9.75209151878078E-008</c:v>
+                  <c:v>8.08067012367249</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.53577471053882E-007</c:v>
+                  <c:v>5.40406853514669</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3.60721763240212E-007</c:v>
+                  <c:v>5.32717563007823</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.87602237563336E-007</c:v>
+                  <c:v>6.01637766168512</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>5.03779757534036E-007</c:v>
+                  <c:v>5.42220436604053</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.02738374710345E-006</c:v>
+                  <c:v>5.06783066641163</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4.01482393098271E-007</c:v>
+                  <c:v>5.84387040638457</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4.55839594802374E-007</c:v>
+                  <c:v>6.7563207761349</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>6.68248365642905E-007</c:v>
+                  <c:v>5.9631636395895</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>8.35736787846614E-007</c:v>
+                  <c:v>7.14037677499423</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>6.94208097740562E-007</c:v>
+                  <c:v>5.38547246699794</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>5.94871845966133E-007</c:v>
+                  <c:v>6.61156570202086</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>8.68648349665587E-007</c:v>
+                  <c:v>6.43992794989476</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>6.60603201006936E-007</c:v>
+                  <c:v>5.30407550143819</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4.72488953293918E-007</c:v>
+                  <c:v>4.76620088223653</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>4.99655414938434E-007</c:v>
+                  <c:v>5.31858260123214</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>4.57995929990185E-007</c:v>
+                  <c:v>4.42190537118259</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>8.32888845412862E-007</c:v>
+                  <c:v>5.7681576052667</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v/>
+                  <c:v>5.66035070862931</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>7.03594517572335E-007</c:v>
+                  <c:v>4.77552071710906</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>7.09844130799086E-007</c:v>
+                  <c:v>4.79805431996423</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>6.94247582030258E-007</c:v>
+                  <c:v>4.08697241434145</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>9.24562112853701E-007</c:v>
+                  <c:v>4.95548823275513</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>5.85661313662649E-007</c:v>
+                  <c:v>4.46802347029649</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>9.82727200247819E-007</c:v>
+                  <c:v>4.75493384700057</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.3916633847961E-006</c:v>
+                  <c:v>5.11245986555183</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>6.91435024579975E-007</c:v>
+                  <c:v>5.03077167788965</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="58122834"/>
-        <c:axId val="49554865"/>
+        <c:axId val="44028610"/>
+        <c:axId val="1474242"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58122834"/>
+        <c:axId val="44028610"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3659,12 +3677,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49554865"/>
+        <c:crossAx val="1474242"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49554865"/>
+        <c:axId val="1474242"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3746,7 +3764,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58122834"/>
+        <c:crossAx val="44028610"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3787,16 +3805,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>141480</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>141840</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>179280</xdr:rowOff>
+      <xdr:rowOff>174960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>241920</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>11520</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3804,8 +3822,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="14755680" y="179280"/>
-        <a:ext cx="5758560" cy="3239640"/>
+        <a:off x="16696080" y="174960"/>
+        <a:ext cx="5757840" cy="2990880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3817,16 +3835,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>910800</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>124560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>68400</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>47520</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>98280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3834,8 +3852,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="14582160" y="3810960"/>
-        <a:ext cx="5758560" cy="3239280"/>
+        <a:off x="16522200" y="3530520"/>
+        <a:ext cx="5758200" cy="3001320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3847,16 +3865,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>26280</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>116280</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>26640</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>153360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>126720</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>134640</xdr:rowOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>150840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3864,8 +3882,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="14640480" y="7308000"/>
-        <a:ext cx="5758560" cy="2856960"/>
+        <a:off x="16580880" y="6776280"/>
+        <a:ext cx="5757840" cy="2646720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3877,16 +3895,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>472320</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>7200</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>472680</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>10080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>569880</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>24840</xdr:rowOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>7200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3894,8 +3912,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15086520" y="10226880"/>
-        <a:ext cx="5755680" cy="2859120"/>
+        <a:off x="17026920" y="9471240"/>
+        <a:ext cx="5754960" cy="2646360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3907,16 +3925,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>443520</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>443880</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>122040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>541080</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>154800</xdr:rowOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>95040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3924,8 +3942,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15057720" y="13405320"/>
-        <a:ext cx="5755680" cy="2858760"/>
+        <a:off x="16998120" y="12421800"/>
+        <a:ext cx="5754960" cy="2629800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3943,25 +3961,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L65536"/>
+  <dimension ref="A1:N67"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B67" activeCellId="0" sqref="B1:B67"/>
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7246963562753"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.4898785425101"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="12" min="9" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -3994,11 +4012,17 @@
       </c>
       <c r="K1" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2583</v>
@@ -4016,28 +4040,36 @@
         <v>656.475468186624</v>
       </c>
       <c r="G2" s="0" t="n">
+        <f aca="false">ABS(E2)</f>
+        <v>0.986940618365878</v>
+      </c>
+      <c r="H2" s="0" t="n">
         <v>0.254152329921264</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="I2" s="0" t="n">
         <v>10.4652483389468</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="J2" s="0" t="n">
         <v>0.00023392485040109</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="K2" s="0" t="n">
         <v>0.000916933166062979</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="L2" s="0" t="n">
+        <f aca="false">K2/B2</f>
+        <v>3.54987675595424E-007</v>
+      </c>
+      <c r="M2" s="0" t="n">
         <v>-915.633833118999</v>
       </c>
-      <c r="L2" s="0" t="n">
-        <f aca="false">J2/B2</f>
-        <v>3.54987675595424E-007</v>
+      <c r="N2" s="1" t="n">
+        <f aca="false">SUM(G2:L2)</f>
+        <v>11.7074925002381</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2599</v>
@@ -4055,28 +4087,36 @@
         <v>737.417683980381</v>
       </c>
       <c r="G3" s="0" t="n">
+        <f aca="false">ABS(E3)</f>
+        <v>0.859589852436386</v>
+      </c>
+      <c r="H3" s="0" t="n">
         <v>0.283731313574599</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="I3" s="0" t="n">
         <v>8.49288502898662</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="J3" s="0" t="n">
         <v>0.000261201826014697</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="K3" s="0" t="n">
         <v>0.000448801686329225</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="L3" s="0" t="n">
+        <f aca="false">K3/B3</f>
+        <v>1.72682449530291E-007</v>
+      </c>
+      <c r="M3" s="0" t="n">
         <v>-913.514787864424</v>
       </c>
-      <c r="L3" s="0" t="n">
-        <f aca="false">J3/B3</f>
-        <v>1.72682449530291E-007</v>
+      <c r="N3" s="1" t="n">
+        <f aca="false">SUM(G3:L3)</f>
+        <v>9.6369163711924</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2612</v>
@@ -4094,28 +4134,36 @@
         <v>666.319909702287</v>
       </c>
       <c r="G4" s="0" t="n">
+        <f aca="false">ABS(E4)</f>
+        <v>0.837826718047012</v>
+      </c>
+      <c r="H4" s="0" t="n">
         <v>0.255099506011595</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="I4" s="0" t="n">
         <v>9.84076549975751</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="J4" s="0" t="n">
         <v>0.000254838590508121</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="K4" s="0" t="n">
         <v>0.00046292557816136</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="L4" s="0" t="n">
+        <f aca="false">K4/B4</f>
+        <v>1.77230313231761E-007</v>
+      </c>
+      <c r="M4" s="0" t="n">
         <v>-911.219665735461</v>
       </c>
-      <c r="L4" s="0" t="n">
-        <f aca="false">J4/B4</f>
-        <v>1.77230313231761E-007</v>
+      <c r="N4" s="1" t="n">
+        <f aca="false">SUM(G4:L4)</f>
+        <v>10.9344096652151</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2623</v>
@@ -4133,28 +4181,36 @@
         <v>688.991392917847</v>
       </c>
       <c r="G5" s="0" t="n">
+        <f aca="false">ABS(E5)</f>
+        <v>0.915592648631872</v>
+      </c>
+      <c r="H5" s="0" t="n">
         <v>0.262673043430365</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="I5" s="0" t="n">
         <v>8.05919687360927</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="J5" s="0" t="n">
         <v>0.000269027108828644</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="K5" s="0" t="n">
         <v>0.000718731985545689</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="L5" s="0" t="n">
+        <f aca="false">K5/B5</f>
+        <v>2.74011431774948E-007</v>
+      </c>
+      <c r="M5" s="0" t="n">
         <v>-904.500916807186</v>
       </c>
-      <c r="L5" s="0" t="n">
-        <f aca="false">J5/B5</f>
-        <v>2.74011431774948E-007</v>
+      <c r="N5" s="1" t="n">
+        <f aca="false">SUM(G5:L5)</f>
+        <v>9.23845059877731</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>2594</v>
@@ -4172,28 +4228,36 @@
         <v>710.143301882933</v>
       </c>
       <c r="G6" s="0" t="n">
+        <f aca="false">ABS(E6)</f>
+        <v>0.723060532640602</v>
+      </c>
+      <c r="H6" s="0" t="n">
         <v>0.273763801805294</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="I6" s="0" t="n">
         <v>5.13243396014153</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="J6" s="0" t="n">
         <v>0.000268173819273147</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="K6" s="0" t="n">
         <v>0.000523851046684099</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="L6" s="0" t="n">
+        <f aca="false">K6/B6</f>
+        <v>2.0194720381037E-007</v>
+      </c>
+      <c r="M6" s="0" t="n">
         <v>-903.488616612666</v>
       </c>
-      <c r="L6" s="0" t="n">
-        <f aca="false">J6/B6</f>
-        <v>2.0194720381037E-007</v>
+      <c r="N6" s="1" t="n">
+        <f aca="false">SUM(G6:L6)</f>
+        <v>6.13005052140059</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2653</v>
@@ -4211,24 +4275,36 @@
         <v>724.009703635211</v>
       </c>
       <c r="G7" s="0" t="n">
+        <f aca="false">ABS(E7)</f>
+        <v>0.913578275926824</v>
+      </c>
+      <c r="H7" s="0" t="n">
         <v>0.272902262960878</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="I7" s="0" t="n">
         <v>8.09572899566172</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="J7" s="0" t="n">
         <v>9.52048619814725E-005</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="K7" s="0" t="n">
         <v>0.00601755923171289</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="L7" s="0" t="n">
+        <f aca="false">K7/B7</f>
+        <v>2.26820928447527E-006</v>
+      </c>
+      <c r="M7" s="0" t="n">
         <v>-900.91104810545</v>
+      </c>
+      <c r="N7" s="1" t="n">
+        <f aca="false">SUM(G7:L7)</f>
+        <v>9.2883245668524</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>2656</v>
@@ -4246,28 +4322,36 @@
         <v>643.035963375194</v>
       </c>
       <c r="G8" s="0" t="n">
+        <f aca="false">ABS(E8)</f>
+        <v>0.763316478237698</v>
+      </c>
+      <c r="H8" s="0" t="n">
         <v>0.242106913921383</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="I8" s="0" t="n">
         <v>4.77090119765199</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="J8" s="0" t="n">
         <v>0.000248174589288792</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="K8" s="0" t="n">
         <v>0.000395735963743339</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="L8" s="0" t="n">
+        <f aca="false">K8/B8</f>
+        <v>1.48996974300956E-007</v>
+      </c>
+      <c r="M8" s="0" t="n">
         <v>-898.928604942916</v>
       </c>
-      <c r="L8" s="0" t="n">
-        <f aca="false">J8/B8</f>
-        <v>1.48996974300956E-007</v>
+      <c r="N8" s="1" t="n">
+        <f aca="false">SUM(G8:L8)</f>
+        <v>5.77696864936108</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2661</v>
@@ -4285,28 +4369,36 @@
         <v>722.250140352385</v>
       </c>
       <c r="G9" s="0" t="n">
+        <f aca="false">ABS(E9)</f>
+        <v>0.893269027626104</v>
+      </c>
+      <c r="H9" s="0" t="n">
         <v>0.271420571346255</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="I9" s="0" t="n">
         <v>9.13855460190578</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="J9" s="0" t="n">
         <v>0.000248809881393702</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="K9" s="0" t="n">
         <v>0.000458906247239853</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="L9" s="0" t="n">
+        <f aca="false">K9/B9</f>
+        <v>1.7245631237875E-007</v>
+      </c>
+      <c r="M9" s="0" t="n">
         <v>-884.4081303076</v>
       </c>
-      <c r="L9" s="0" t="n">
-        <f aca="false">J9/B9</f>
-        <v>1.7245631237875E-007</v>
+      <c r="N9" s="1" t="n">
+        <f aca="false">SUM(G9:L9)</f>
+        <v>10.3039520894631</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2691</v>
@@ -4324,28 +4416,36 @@
         <v>747.930332632181</v>
       </c>
       <c r="G10" s="0" t="n">
+        <f aca="false">ABS(E10)</f>
+        <v>1.0301452627925</v>
+      </c>
+      <c r="H10" s="0" t="n">
         <v>0.277937693285835</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="I10" s="0" t="n">
         <v>6.05820527174251</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="J10" s="0" t="n">
         <v>0.000250673704680539</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="K10" s="0" t="n">
         <v>0.000475068864701</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="L10" s="0" t="n">
+        <f aca="false">K10/B10</f>
+        <v>1.76539897696395E-007</v>
+      </c>
+      <c r="M10" s="0" t="n">
         <v>-862.41524984676</v>
       </c>
-      <c r="L10" s="0" t="n">
-        <f aca="false">J10/B10</f>
-        <v>1.76539897696395E-007</v>
+      <c r="N10" s="1" t="n">
+        <f aca="false">SUM(G10:L10)</f>
+        <v>7.36701414693012</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>2772</v>
@@ -4363,28 +4463,36 @@
         <v>739.323809375523</v>
       </c>
       <c r="G11" s="0" t="n">
+        <f aca="false">ABS(E11)</f>
+        <v>0.825540571779158</v>
+      </c>
+      <c r="H11" s="0" t="n">
         <v>0.266711330943551</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="I11" s="0" t="n">
         <v>5.39877277432953</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="J11" s="0" t="n">
         <v>0.000231316283571329</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="K11" s="0" t="n">
         <v>0.00106486951089992</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="L11" s="0" t="n">
+        <f aca="false">K11/B11</f>
+        <v>3.84152060209206E-007</v>
+      </c>
+      <c r="M11" s="0" t="n">
         <v>-835.517463070681</v>
       </c>
-      <c r="L11" s="0" t="n">
-        <f aca="false">J11/B11</f>
-        <v>3.84152060209206E-007</v>
+      <c r="N11" s="1" t="n">
+        <f aca="false">SUM(G11:L11)</f>
+        <v>6.49232124699877</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>2792</v>
@@ -4402,28 +4510,36 @@
         <v>684.282507455267</v>
       </c>
       <c r="G12" s="0" t="n">
+        <f aca="false">ABS(E12)</f>
+        <v>0.767418410457992</v>
+      </c>
+      <c r="H12" s="0" t="n">
         <v>0.245086857971084</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="I12" s="0" t="n">
         <v>6.94393229425373</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="J12" s="0" t="n">
         <v>0.000259724864981171</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="K12" s="0" t="n">
         <v>0.000503867076445392</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="L12" s="0" t="n">
+        <f aca="false">K12/B12</f>
+        <v>1.80468150589324E-007</v>
+      </c>
+      <c r="M12" s="0" t="n">
         <v>-810.968114001913</v>
       </c>
-      <c r="L12" s="0" t="n">
-        <f aca="false">J12/B12</f>
-        <v>1.80468150589324E-007</v>
+      <c r="N12" s="1" t="n">
+        <f aca="false">SUM(G12:L12)</f>
+        <v>7.95720133509238</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>2829</v>
@@ -4441,28 +4557,36 @@
         <v>669.372795732482</v>
       </c>
       <c r="G13" s="0" t="n">
+        <f aca="false">ABS(E13)</f>
+        <v>0.950632181943604</v>
+      </c>
+      <c r="H13" s="0" t="n">
         <v>0.236611097819895</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="I13" s="0" t="n">
         <v>7.0450922599729</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="J13" s="0" t="n">
         <v>0.000246550761062776</v>
       </c>
-      <c r="J13" s="0" t="n">
+      <c r="K13" s="0" t="n">
         <v>0.000486295791254046</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="L13" s="0" t="n">
+        <f aca="false">K13/B13</f>
+        <v>1.71896709527765E-007</v>
+      </c>
+      <c r="M13" s="0" t="n">
         <v>-790.779455100395</v>
       </c>
-      <c r="L13" s="0" t="n">
-        <f aca="false">J13/B13</f>
-        <v>1.71896709527765E-007</v>
+      <c r="N13" s="1" t="n">
+        <f aca="false">SUM(G13:L13)</f>
+        <v>8.23306855818543</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>2913</v>
@@ -4480,28 +4604,36 @@
         <v>664.828772047107</v>
       </c>
       <c r="G14" s="0" t="n">
+        <f aca="false">ABS(E14)</f>
+        <v>0.823951551208182</v>
+      </c>
+      <c r="H14" s="0" t="n">
         <v>0.228228208735704</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="I14" s="0" t="n">
         <v>5.69048933386173</v>
       </c>
-      <c r="I14" s="0" t="n">
+      <c r="J14" s="0" t="n">
         <v>0.000242995731457741</v>
       </c>
-      <c r="J14" s="0" t="n">
+      <c r="K14" s="0" t="n">
         <v>0.000432601575954628</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="L14" s="0" t="n">
+        <f aca="false">K14/B14</f>
+        <v>1.48507235137188E-007</v>
+      </c>
+      <c r="M14" s="0" t="n">
         <v>-782.004415146655</v>
       </c>
-      <c r="L14" s="0" t="n">
-        <f aca="false">J14/B14</f>
-        <v>1.48507235137188E-007</v>
+      <c r="N14" s="1" t="n">
+        <f aca="false">SUM(G14:L14)</f>
+        <v>6.74334483962026</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>2865</v>
@@ -4519,28 +4651,36 @@
         <v>717.215267590177</v>
       </c>
       <c r="G15" s="0" t="n">
+        <f aca="false">ABS(E15)</f>
+        <v>0.841482165257958</v>
+      </c>
+      <c r="H15" s="0" t="n">
         <v>0.250336917134442</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="I15" s="0" t="n">
         <v>27.3335815244418</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="J15" s="0" t="n">
         <v>0.00024971808926392</v>
       </c>
-      <c r="J15" s="0" t="n">
+      <c r="K15" s="0" t="n">
         <v>0.000486955263572127</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="L15" s="0" t="n">
+        <f aca="false">K15/B15</f>
+        <v>1.69966933183989E-007</v>
+      </c>
+      <c r="M15" s="0" t="n">
         <v>-780.755162674451</v>
       </c>
-      <c r="L15" s="0" t="n">
-        <f aca="false">J15/B15</f>
-        <v>1.69966933183989E-007</v>
+      <c r="N15" s="1" t="n">
+        <f aca="false">SUM(G15:L15)</f>
+        <v>28.426137450154</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>2877</v>
@@ -4558,28 +4698,36 @@
         <v>711.505049893501</v>
       </c>
       <c r="G16" s="0" t="n">
+        <f aca="false">ABS(E16)</f>
+        <v>1.03125161820404</v>
+      </c>
+      <c r="H16" s="0" t="n">
         <v>0.247307977022419</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="I16" s="0" t="n">
         <v>8.54282010178537</v>
       </c>
-      <c r="I16" s="0" t="n">
+      <c r="J16" s="0" t="n">
         <v>0.000246392185137966</v>
       </c>
-      <c r="J16" s="0" t="n">
+      <c r="K16" s="0" t="n">
         <v>0.000457307394329213</v>
       </c>
-      <c r="K16" s="0" t="n">
+      <c r="L16" s="0" t="n">
+        <f aca="false">K16/B16</f>
+        <v>1.58952865599309E-007</v>
+      </c>
+      <c r="M16" s="0" t="n">
         <v>-778.636828530828</v>
       </c>
-      <c r="L16" s="0" t="n">
-        <f aca="false">J16/B16</f>
-        <v>1.58952865599309E-007</v>
+      <c r="N16" s="1" t="n">
+        <f aca="false">SUM(G16:L16)</f>
+        <v>9.82208355554416</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>2879</v>
@@ -4597,28 +4745,36 @@
         <v>641.892212053591</v>
       </c>
       <c r="G17" s="0" t="n">
+        <f aca="false">ABS(E17)</f>
+        <v>0.988388530148484</v>
+      </c>
+      <c r="H17" s="0" t="n">
         <v>0.222956655801872</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="I17" s="0" t="n">
         <v>4.77094000437745</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="J17" s="0" t="n">
         <v>0.000238171997955881</v>
       </c>
-      <c r="J17" s="0" t="n">
+      <c r="K17" s="0" t="n">
         <v>0.000425302874912865</v>
       </c>
-      <c r="K17" s="0" t="n">
+      <c r="L17" s="0" t="n">
+        <f aca="false">K17/B17</f>
+        <v>1.47725903061085E-007</v>
+      </c>
+      <c r="M17" s="0" t="n">
         <v>-778.495824114239</v>
       </c>
-      <c r="L17" s="0" t="n">
-        <f aca="false">J17/B17</f>
-        <v>1.47725903061085E-007</v>
+      <c r="N17" s="1" t="n">
+        <f aca="false">SUM(G17:L17)</f>
+        <v>5.98294881292658</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>2924</v>
@@ -4636,28 +4792,36 @@
         <v>700.82143329526</v>
       </c>
       <c r="G18" s="0" t="n">
+        <f aca="false">ABS(E18)</f>
+        <v>1.02422330402121</v>
+      </c>
+      <c r="H18" s="0" t="n">
         <v>0.239679012754877</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="I18" s="0" t="n">
         <v>5.09988011555987</v>
       </c>
-      <c r="I18" s="0" t="n">
+      <c r="J18" s="0" t="n">
         <v>0.000234963726236403</v>
       </c>
-      <c r="J18" s="0" t="n">
+      <c r="K18" s="0" t="n">
         <v>0.000380736092612812</v>
       </c>
-      <c r="K18" s="0" t="n">
+      <c r="L18" s="0" t="n">
+        <f aca="false">K18/B18</f>
+        <v>1.30210701987966E-007</v>
+      </c>
+      <c r="M18" s="0" t="n">
         <v>-777.416923436149</v>
       </c>
-      <c r="L18" s="0" t="n">
-        <f aca="false">J18/B18</f>
-        <v>1.30210701987966E-007</v>
+      <c r="N18" s="1" t="n">
+        <f aca="false">SUM(G18:L18)</f>
+        <v>6.36439826236551</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>2898</v>
@@ -4675,28 +4839,36 @@
         <v>684.707044108237</v>
       </c>
       <c r="G19" s="0" t="n">
+        <f aca="false">ABS(E19)</f>
+        <v>0.848741652227773</v>
+      </c>
+      <c r="H19" s="0" t="n">
         <v>0.236268821293387</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="I19" s="0" t="n">
         <v>4.42600268908882</v>
       </c>
-      <c r="I19" s="0" t="n">
+      <c r="J19" s="0" t="n">
         <v>0.000241614003011567</v>
       </c>
-      <c r="J19" s="0" t="n">
+      <c r="K19" s="0" t="n">
         <v>0.000400515729168809</v>
       </c>
-      <c r="K19" s="0" t="n">
+      <c r="L19" s="0" t="n">
+        <f aca="false">K19/B19</f>
+        <v>1.38204185358457E-007</v>
+      </c>
+      <c r="M19" s="0" t="n">
         <v>-776.152222237845</v>
       </c>
-      <c r="L19" s="0" t="n">
-        <f aca="false">J19/B19</f>
-        <v>1.38204185358457E-007</v>
+      <c r="N19" s="1" t="n">
+        <f aca="false">SUM(G19:L19)</f>
+        <v>5.51165543054635</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>2868</v>
@@ -4714,28 +4886,36 @@
         <v>671.573949630681</v>
       </c>
       <c r="G20" s="0" t="n">
+        <f aca="false">ABS(E20)</f>
+        <v>0.959430043416518</v>
+      </c>
+      <c r="H20" s="0" t="n">
         <v>0.234161070303585</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="I20" s="0" t="n">
         <v>6.0739425806583</v>
       </c>
-      <c r="I20" s="0" t="n">
+      <c r="J20" s="0" t="n">
         <v>0.000234416380589915</v>
       </c>
-      <c r="J20" s="0" t="n">
+      <c r="K20" s="0" t="n">
         <v>0.000405189669854725</v>
       </c>
-      <c r="K20" s="0" t="n">
+      <c r="L20" s="0" t="n">
+        <f aca="false">K20/B20</f>
+        <v>1.41279522264548E-007</v>
+      </c>
+      <c r="M20" s="0" t="n">
         <v>-775.472479847163</v>
       </c>
-      <c r="L20" s="0" t="n">
-        <f aca="false">J20/B20</f>
-        <v>1.41279522264548E-007</v>
+      <c r="N20" s="1" t="n">
+        <f aca="false">SUM(G20:L20)</f>
+        <v>7.26817344170837</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>2905</v>
@@ -4753,28 +4933,36 @@
         <v>633.792167476907</v>
       </c>
       <c r="G21" s="0" t="n">
+        <f aca="false">ABS(E21)</f>
+        <v>0.839247773607639</v>
+      </c>
+      <c r="H21" s="0" t="n">
         <v>0.218172863159004</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="I21" s="0" t="n">
         <v>5.33691196223685</v>
       </c>
-      <c r="I21" s="0" t="n">
+      <c r="J21" s="0" t="n">
         <v>0.000235135976747504</v>
       </c>
-      <c r="J21" s="0" t="n">
+      <c r="K21" s="0" t="n">
         <v>0.000372653108103866</v>
       </c>
-      <c r="K21" s="0" t="n">
+      <c r="L21" s="0" t="n">
+        <f aca="false">K21/B21</f>
+        <v>1.28279899519403E-007</v>
+      </c>
+      <c r="M21" s="0" t="n">
         <v>-771.407643293807</v>
       </c>
-      <c r="L21" s="0" t="n">
-        <f aca="false">J21/B21</f>
-        <v>1.28279899519403E-007</v>
+      <c r="N21" s="1" t="n">
+        <f aca="false">SUM(G21:L21)</f>
+        <v>6.39494051636824</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>2959</v>
@@ -4792,28 +4980,36 @@
         <v>664.993478419549</v>
       </c>
       <c r="G22" s="0" t="n">
+        <f aca="false">ABS(E22)</f>
+        <v>0.922533589093121</v>
+      </c>
+      <c r="H22" s="0" t="n">
         <v>0.224735883210392</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="I22" s="0" t="n">
         <v>4.95800748504766</v>
       </c>
-      <c r="I22" s="0" t="n">
+      <c r="J22" s="0" t="n">
         <v>0.00023236782836713</v>
       </c>
-      <c r="J22" s="0" t="n">
+      <c r="K22" s="0" t="n">
         <v>0.000343100171990744</v>
       </c>
-      <c r="K22" s="0" t="n">
+      <c r="L22" s="0" t="n">
+        <f aca="false">K22/B22</f>
+        <v>1.15951393035061E-007</v>
+      </c>
+      <c r="M22" s="0" t="n">
         <v>-756.174487389124</v>
       </c>
-      <c r="L22" s="0" t="n">
-        <f aca="false">J22/B22</f>
-        <v>1.15951393035061E-007</v>
+      <c r="N22" s="1" t="n">
+        <f aca="false">SUM(G22:L22)</f>
+        <v>6.10585254130293</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>3032</v>
@@ -4831,28 +5027,36 @@
         <v>643.381766430941</v>
       </c>
       <c r="G23" s="0" t="n">
+        <f aca="false">ABS(E23)</f>
+        <v>0.946839057348683</v>
+      </c>
+      <c r="H23" s="0" t="n">
         <v>0.212197152516801</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="I23" s="0" t="n">
         <v>3.68918927874373</v>
       </c>
-      <c r="I23" s="0" t="n">
+      <c r="J23" s="0" t="n">
         <v>0.000230778328030802</v>
       </c>
-      <c r="J23" s="0" t="n">
+      <c r="K23" s="0" t="n">
         <v>0.000364458403742308</v>
       </c>
-      <c r="K23" s="0" t="n">
+      <c r="L23" s="0" t="n">
+        <f aca="false">K23/B23</f>
+        <v>1.20203959017912E-007</v>
+      </c>
+      <c r="M23" s="0" t="n">
         <v>-721.702547139754</v>
       </c>
-      <c r="L23" s="0" t="n">
-        <f aca="false">J23/B23</f>
-        <v>1.20203959017912E-007</v>
+      <c r="N23" s="1" t="n">
+        <f aca="false">SUM(G23:L23)</f>
+        <v>4.84882084554495</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>3264</v>
@@ -4870,28 +5074,36 @@
         <v>643.589671791135</v>
       </c>
       <c r="G24" s="0" t="n">
+        <f aca="false">ABS(E24)</f>
+        <v>0.997675397203579</v>
+      </c>
+      <c r="H24" s="0" t="n">
         <v>0.197178208269343</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="I24" s="0" t="n">
         <v>3.45689124434529</v>
       </c>
-      <c r="I24" s="0" t="n">
+      <c r="J24" s="0" t="n">
         <v>0.000218216707699902</v>
       </c>
-      <c r="J24" s="0" t="n">
+      <c r="K24" s="0" t="n">
         <v>0.000330931040398398</v>
       </c>
-      <c r="K24" s="0" t="n">
+      <c r="L24" s="0" t="n">
+        <f aca="false">K24/B24</f>
+        <v>1.01388186396568E-007</v>
+      </c>
+      <c r="M24" s="0" t="n">
         <v>-628.115714441663</v>
       </c>
-      <c r="L24" s="0" t="n">
-        <f aca="false">J24/B24</f>
-        <v>1.01388186396568E-007</v>
+      <c r="N24" s="1" t="n">
+        <f aca="false">SUM(G24:L24)</f>
+        <v>4.6522940989545</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>3407</v>
@@ -4909,28 +5121,36 @@
         <v>632.666625970629</v>
       </c>
       <c r="G25" s="0" t="n">
+        <f aca="false">ABS(E25)</f>
+        <v>0.875300178536975</v>
+      </c>
+      <c r="H25" s="0" t="n">
         <v>0.185696103895107</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="I25" s="0" t="n">
         <v>4.30131134878275</v>
       </c>
-      <c r="I25" s="0" t="n">
+      <c r="J25" s="0" t="n">
         <v>0.000213768031858265</v>
       </c>
-      <c r="J25" s="0" t="n">
+      <c r="K25" s="0" t="n">
         <v>0.00026912355508231</v>
       </c>
-      <c r="K25" s="0" t="n">
+      <c r="L25" s="0" t="n">
+        <f aca="false">K25/B25</f>
+        <v>7.89913575234253E-008</v>
+      </c>
+      <c r="M25" s="0" t="n">
         <v>-576.273584945456</v>
       </c>
-      <c r="L25" s="0" t="n">
-        <f aca="false">J25/B25</f>
-        <v>7.89913575234253E-008</v>
+      <c r="N25" s="1" t="n">
+        <f aca="false">SUM(G25:L25)</f>
+        <v>5.36279060179313</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>3531</v>
@@ -4948,28 +5168,36 @@
         <v>686.390610877499</v>
       </c>
       <c r="G26" s="0" t="n">
+        <f aca="false">ABS(E26)</f>
+        <v>0.923580149638866</v>
+      </c>
+      <c r="H26" s="0" t="n">
         <v>0.194389864309685</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="I26" s="0" t="n">
         <v>4.20068243162049</v>
       </c>
-      <c r="I26" s="0" t="n">
+      <c r="J26" s="0" t="n">
         <v>0.000212968465016718</v>
       </c>
-      <c r="J26" s="0" t="n">
+      <c r="K26" s="0" t="n">
         <v>0.000264287785175412</v>
       </c>
-      <c r="K26" s="0" t="n">
+      <c r="L26" s="0" t="n">
+        <f aca="false">K26/B26</f>
+        <v>7.48478575971147E-008</v>
+      </c>
+      <c r="M26" s="0" t="n">
         <v>-528.184282586059</v>
       </c>
-      <c r="L26" s="0" t="n">
-        <f aca="false">J26/B26</f>
-        <v>7.48478575971147E-008</v>
+      <c r="N26" s="1" t="n">
+        <f aca="false">SUM(G26:L26)</f>
+        <v>5.31912977666709</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>3770</v>
@@ -4987,28 +5215,36 @@
         <v>617.486606381091</v>
       </c>
       <c r="G27" s="0" t="n">
+        <f aca="false">ABS(E27)</f>
+        <v>0.889768704339502</v>
+      </c>
+      <c r="H27" s="0" t="n">
         <v>0.163789550764215</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="I27" s="0" t="n">
         <v>3.4846091300696</v>
       </c>
-      <c r="I27" s="0" t="n">
+      <c r="J27" s="0" t="n">
         <v>0.000205366312609069</v>
       </c>
-      <c r="J27" s="0" t="n">
+      <c r="K27" s="0" t="n">
         <v>0.000217043194255187</v>
       </c>
-      <c r="K27" s="0" t="n">
+      <c r="L27" s="0" t="n">
+        <f aca="false">K27/B27</f>
+        <v>5.75711390597313E-008</v>
+      </c>
+      <c r="M27" s="0" t="n">
         <v>-443.857237441114</v>
       </c>
-      <c r="L27" s="0" t="n">
-        <f aca="false">J27/B27</f>
-        <v>5.75711390597313E-008</v>
+      <c r="N27" s="1" t="n">
+        <f aca="false">SUM(G27:L27)</f>
+        <v>4.53858985225132</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>3950</v>
@@ -5026,28 +5262,36 @@
         <v>619.620451205686</v>
       </c>
       <c r="G28" s="0" t="n">
+        <f aca="false">ABS(E28)</f>
+        <v>0.942217834871201</v>
+      </c>
+      <c r="H28" s="0" t="n">
         <v>0.156865937014098</v>
       </c>
-      <c r="H28" s="0" t="n">
+      <c r="I28" s="0" t="n">
         <v>5.78101861605353</v>
       </c>
-      <c r="I28" s="0" t="n">
+      <c r="J28" s="0" t="n">
         <v>0.000207016412493615</v>
       </c>
-      <c r="J28" s="0" t="n">
+      <c r="K28" s="0" t="n">
         <v>0.00022948951692887</v>
       </c>
-      <c r="K28" s="0" t="n">
+      <c r="L28" s="0" t="n">
+        <f aca="false">K28/B28</f>
+        <v>5.80986118807266E-008</v>
+      </c>
+      <c r="M28" s="0" t="n">
         <v>-397.503525883761</v>
       </c>
-      <c r="L28" s="0" t="n">
-        <f aca="false">J28/B28</f>
-        <v>5.80986118807266E-008</v>
+      <c r="N28" s="1" t="n">
+        <f aca="false">SUM(G28:L28)</f>
+        <v>6.88053895196686</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>4162</v>
@@ -5065,28 +5309,36 @@
         <v>715.522989390263</v>
       </c>
       <c r="G29" s="0" t="n">
+        <f aca="false">ABS(E29)</f>
+        <v>0.947725445354394</v>
+      </c>
+      <c r="H29" s="0" t="n">
         <v>0.171918065687233</v>
       </c>
-      <c r="H29" s="0" t="n">
+      <c r="I29" s="0" t="n">
         <v>6.30932127014074</v>
       </c>
-      <c r="I29" s="0" t="n">
+      <c r="J29" s="0" t="n">
         <v>0.000215465772851879</v>
       </c>
-      <c r="J29" s="0" t="n">
+      <c r="K29" s="0" t="n">
         <v>0.000302838102925842</v>
       </c>
-      <c r="K29" s="0" t="n">
+      <c r="L29" s="0" t="n">
+        <f aca="false">K29/B29</f>
+        <v>7.27626388577227E-008</v>
+      </c>
+      <c r="M29" s="0" t="n">
         <v>-333.981925008314</v>
       </c>
-      <c r="L29" s="0" t="n">
-        <f aca="false">J29/B29</f>
-        <v>7.27626388577227E-008</v>
+      <c r="N29" s="1" t="n">
+        <f aca="false">SUM(G29:L29)</f>
+        <v>7.42948315782078</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>4444</v>
@@ -5104,28 +5356,36 @@
         <v>757.866620792873</v>
       </c>
       <c r="G30" s="0" t="n">
+        <f aca="false">ABS(E30)</f>
+        <v>1.00907076644697</v>
+      </c>
+      <c r="H30" s="0" t="n">
         <v>0.170537043382735</v>
       </c>
-      <c r="H30" s="0" t="n">
+      <c r="I30" s="0" t="n">
         <v>3.89895447638196</v>
       </c>
-      <c r="I30" s="0" t="n">
+      <c r="J30" s="0" t="n">
         <v>0.000207457017257461</v>
       </c>
-      <c r="J30" s="0" t="n">
+      <c r="K30" s="0" t="n">
         <v>0.000240932960224851</v>
       </c>
-      <c r="K30" s="0" t="n">
+      <c r="L30" s="0" t="n">
+        <f aca="false">K30/B30</f>
+        <v>5.42153375843499E-008</v>
+      </c>
+      <c r="M30" s="0" t="n">
         <v>-255.402412665557</v>
       </c>
-      <c r="L30" s="0" t="n">
-        <f aca="false">J30/B30</f>
-        <v>5.42153375843499E-008</v>
+      <c r="N30" s="1" t="n">
+        <f aca="false">SUM(G30:L30)</f>
+        <v>5.07901073040449</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>4806</v>
@@ -5143,28 +5403,36 @@
         <v>783.023611214356</v>
       </c>
       <c r="G31" s="0" t="n">
+        <f aca="false">ABS(E31)</f>
+        <v>0.961650690467707</v>
+      </c>
+      <c r="H31" s="0" t="n">
         <v>0.16292626117652</v>
       </c>
-      <c r="H31" s="0" t="n">
+      <c r="I31" s="0" t="n">
         <v>2.60536838788374</v>
       </c>
-      <c r="I31" s="0" t="n">
+      <c r="J31" s="0" t="n">
         <v>0.000211628359523288</v>
       </c>
-      <c r="J31" s="0" t="n">
+      <c r="K31" s="0" t="n">
         <v>0.000269999987793332</v>
       </c>
-      <c r="K31" s="0" t="n">
+      <c r="L31" s="0" t="n">
+        <f aca="false">K31/B31</f>
+        <v>5.61797727410179E-008</v>
+      </c>
+      <c r="M31" s="0" t="n">
         <v>-178.722012234352</v>
       </c>
-      <c r="L31" s="0" t="n">
-        <f aca="false">J31/B31</f>
-        <v>5.61797727410179E-008</v>
+      <c r="N31" s="1" t="n">
+        <f aca="false">SUM(G31:L31)</f>
+        <v>3.73042702405506</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>5112</v>
@@ -5182,28 +5450,36 @@
         <v>855.271709449415</v>
       </c>
       <c r="G32" s="0" t="n">
+        <f aca="false">ABS(E32)</f>
+        <v>0.910893809951546</v>
+      </c>
+      <c r="H32" s="0" t="n">
         <v>0.167306672427507</v>
       </c>
-      <c r="H32" s="0" t="n">
+      <c r="I32" s="0" t="n">
         <v>6.30902957005191</v>
       </c>
-      <c r="I32" s="0" t="n">
+      <c r="J32" s="0" t="n">
         <v>0.000235364758419735</v>
       </c>
-      <c r="J32" s="0" t="n">
+      <c r="K32" s="0" t="n">
         <v>0.000929809256086311</v>
       </c>
-      <c r="K32" s="0" t="n">
+      <c r="L32" s="0" t="n">
+        <f aca="false">K32/B32</f>
+        <v>1.81887569656947E-007</v>
+      </c>
+      <c r="M32" s="0" t="n">
         <v>-113.076603811607</v>
       </c>
-      <c r="L32" s="0" t="n">
-        <f aca="false">J32/B32</f>
-        <v>1.81887569656947E-007</v>
+      <c r="N32" s="1" t="n">
+        <f aca="false">SUM(G32:L32)</f>
+        <v>7.38839540833304</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>5436</v>
@@ -5221,28 +5497,36 @@
         <v>845.523643252822</v>
       </c>
       <c r="G33" s="0" t="n">
+        <f aca="false">ABS(E33)</f>
+        <v>0.879524251417905</v>
+      </c>
+      <c r="H33" s="0" t="n">
         <v>0.15554150906049</v>
       </c>
-      <c r="H33" s="0" t="n">
+      <c r="I33" s="0" t="n">
         <v>4.73791161802097</v>
       </c>
-      <c r="I33" s="0" t="n">
+      <c r="J33" s="0" t="n">
         <v>0.000216420753479473</v>
       </c>
-      <c r="J33" s="0" t="n">
+      <c r="K33" s="0" t="n">
         <v>0.000407612421108503</v>
       </c>
-      <c r="K33" s="0" t="n">
+      <c r="L33" s="0" t="n">
+        <f aca="false">K33/B33</f>
+        <v>7.49838890928078E-008</v>
+      </c>
+      <c r="M33" s="0" t="n">
         <v>-56.1081751651907</v>
       </c>
-      <c r="L33" s="0" t="n">
-        <f aca="false">J33/B33</f>
-        <v>7.49838890928078E-008</v>
+      <c r="N33" s="1" t="n">
+        <f aca="false">SUM(G33:L33)</f>
+        <v>5.77360148665784</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>5647</v>
@@ -5260,28 +5544,36 @@
         <v>846.746132765401</v>
       </c>
       <c r="G34" s="0" t="n">
+        <f aca="false">ABS(E34)</f>
+        <v>0.867231061585812</v>
+      </c>
+      <c r="H34" s="0" t="n">
         <v>0.149946189616682</v>
       </c>
-      <c r="H34" s="0" t="n">
+      <c r="I34" s="0" t="n">
         <v>3.75795746713254</v>
       </c>
-      <c r="I34" s="0" t="n">
+      <c r="J34" s="0" t="n">
         <v>0.000201369121405636</v>
       </c>
-      <c r="J34" s="0" t="n">
+      <c r="K34" s="0" t="n">
         <v>0.000199144595361659</v>
       </c>
-      <c r="K34" s="0" t="n">
+      <c r="L34" s="0" t="n">
+        <f aca="false">K34/B34</f>
+        <v>3.52655561115033E-008</v>
+      </c>
+      <c r="M34" s="0" t="n">
         <v>-7.23067478259313</v>
       </c>
-      <c r="L34" s="0" t="n">
-        <f aca="false">J34/B34</f>
-        <v>3.52655561115033E-008</v>
+      <c r="N34" s="1" t="n">
+        <f aca="false">SUM(G34:L34)</f>
+        <v>4.77553526731736</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>5980</v>
@@ -5299,28 +5591,36 @@
         <v>870.216370975291</v>
       </c>
       <c r="G35" s="0" t="n">
+        <f aca="false">ABS(E35)</f>
+        <v>0.844443395254558</v>
+      </c>
+      <c r="H35" s="0" t="n">
         <v>0.145521132270116</v>
       </c>
-      <c r="H35" s="0" t="n">
+      <c r="I35" s="0" t="n">
         <v>4.22256615139975</v>
       </c>
-      <c r="I35" s="0" t="n">
+      <c r="J35" s="0" t="n">
         <v>0.000200334793966403</v>
       </c>
-      <c r="J35" s="0" t="n">
+      <c r="K35" s="0" t="n">
         <v>0.00019472334197852</v>
       </c>
-      <c r="K35" s="0" t="n">
+      <c r="L35" s="0" t="n">
+        <f aca="false">K35/B35</f>
+        <v>3.25624317689833E-008</v>
+      </c>
+      <c r="M35" s="0" t="n">
         <v>44.0173311043849</v>
       </c>
-      <c r="L35" s="0" t="n">
-        <f aca="false">J35/B35</f>
-        <v>3.25624317689833E-008</v>
+      <c r="N35" s="1" t="n">
+        <f aca="false">SUM(G35:L35)</f>
+        <v>5.2129257696228</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>6283</v>
@@ -5338,28 +5638,36 @@
         <v>961.587385380612</v>
       </c>
       <c r="G36" s="0" t="n">
+        <f aca="false">ABS(E36)</f>
+        <v>0.803643714351239</v>
+      </c>
+      <c r="H36" s="0" t="n">
         <v>0.153045899312528</v>
       </c>
-      <c r="H36" s="0" t="n">
+      <c r="I36" s="0" t="n">
         <v>13.5077281107611</v>
       </c>
-      <c r="I36" s="0" t="n">
+      <c r="J36" s="0" t="n">
         <v>0.000200225770713309</v>
       </c>
-      <c r="J36" s="0" t="n">
+      <c r="K36" s="0" t="n">
         <v>0.000185022166966056</v>
       </c>
-      <c r="K36" s="0" t="n">
+      <c r="L36" s="0" t="n">
+        <f aca="false">K36/B36</f>
+        <v>2.94480609527385E-008</v>
+      </c>
+      <c r="M36" s="0" t="n">
         <v>99.2120862986552</v>
       </c>
-      <c r="L36" s="0" t="n">
-        <f aca="false">J36/B36</f>
-        <v>2.94480609527385E-008</v>
+      <c r="N36" s="1" t="n">
+        <f aca="false">SUM(G36:L36)</f>
+        <v>14.4648030018106</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>6986</v>
@@ -5377,28 +5685,36 @@
         <v>1077.42510724939</v>
       </c>
       <c r="G37" s="0" t="n">
+        <f aca="false">ABS(E37)</f>
+        <v>0.777328733094066</v>
+      </c>
+      <c r="H37" s="0" t="n">
         <v>0.154226325114427</v>
       </c>
-      <c r="H37" s="0" t="n">
+      <c r="I37" s="0" t="n">
         <v>3.67123387771807</v>
       </c>
-      <c r="I37" s="0" t="n">
+      <c r="J37" s="0" t="n">
         <v>0.0002203414412544</v>
       </c>
-      <c r="J37" s="0" t="n">
+      <c r="K37" s="0" t="n">
         <v>0.000320824054754699</v>
       </c>
-      <c r="K37" s="0" t="n">
+      <c r="L37" s="0" t="n">
+        <f aca="false">K37/B37</f>
+        <v>4.59238555331662E-008</v>
+      </c>
+      <c r="M37" s="0" t="n">
         <v>209.798452996868</v>
       </c>
-      <c r="L37" s="0" t="n">
-        <f aca="false">J37/B37</f>
-        <v>4.59238555331662E-008</v>
+      <c r="N37" s="1" t="n">
+        <f aca="false">SUM(G37:L37)</f>
+        <v>4.60333014734643</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>7374</v>
@@ -5416,28 +5732,36 @@
         <v>1213.51272919199</v>
       </c>
       <c r="G38" s="0" t="n">
+        <f aca="false">ABS(E38)</f>
+        <v>0.801034810956338</v>
+      </c>
+      <c r="H38" s="0" t="n">
         <v>0.164566412963384</v>
       </c>
-      <c r="H38" s="0" t="n">
+      <c r="I38" s="0" t="n">
         <v>4.48470224541995</v>
       </c>
-      <c r="I38" s="0" t="n">
+      <c r="J38" s="0" t="n">
         <v>0.000249790306558463</v>
       </c>
-      <c r="J38" s="0" t="n">
+      <c r="K38" s="0" t="n">
         <v>0.000833162971436388</v>
       </c>
-      <c r="K38" s="0" t="n">
+      <c r="L38" s="0" t="n">
+        <f aca="false">K38/B38</f>
+        <v>1.12986570577216E-007</v>
+      </c>
+      <c r="M38" s="0" t="n">
         <v>257.242977178053</v>
       </c>
-      <c r="L38" s="0" t="n">
-        <f aca="false">J38/B38</f>
-        <v>1.12986570577216E-007</v>
+      <c r="N38" s="1" t="n">
+        <f aca="false">SUM(G38:L38)</f>
+        <v>5.45138653560424</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>7722</v>
@@ -5455,28 +5779,36 @@
         <v>1302.4272380397</v>
       </c>
       <c r="G39" s="0" t="n">
+        <f aca="false">ABS(E39)</f>
+        <v>0.747285591884605</v>
+      </c>
+      <c r="H39" s="0" t="n">
         <v>0.168664495990638</v>
       </c>
-      <c r="H39" s="0" t="n">
+      <c r="I39" s="0" t="n">
         <v>4.19604448762831</v>
       </c>
-      <c r="I39" s="0" t="n">
+      <c r="J39" s="0" t="n">
         <v>0.00027784633651049</v>
       </c>
-      <c r="J39" s="0" t="n">
+      <c r="K39" s="0" t="n">
         <v>0.000911958251353555</v>
       </c>
-      <c r="K39" s="0" t="n">
+      <c r="L39" s="0" t="n">
+        <f aca="false">K39/B39</f>
+        <v>1.18098711648997E-007</v>
+      </c>
+      <c r="M39" s="0" t="n">
         <v>296.141174817834</v>
       </c>
-      <c r="L39" s="0" t="n">
-        <f aca="false">J39/B39</f>
-        <v>1.18098711648997E-007</v>
+      <c r="N39" s="1" t="n">
+        <f aca="false">SUM(G39:L39)</f>
+        <v>5.11318449819013</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>8025</v>
@@ -5494,28 +5826,36 @@
         <v>1376.82554598252</v>
       </c>
       <c r="G40" s="0" t="n">
+        <f aca="false">ABS(E40)</f>
+        <v>0.731516002038831</v>
+      </c>
+      <c r="H40" s="0" t="n">
         <v>0.171567046228351</v>
       </c>
-      <c r="H40" s="0" t="n">
+      <c r="I40" s="0" t="n">
         <v>8.15006752369865</v>
       </c>
-      <c r="I40" s="0" t="n">
+      <c r="J40" s="0" t="n">
         <v>0.00036893636704492</v>
       </c>
-      <c r="J40" s="0" t="n">
+      <c r="K40" s="0" t="n">
         <v>0.00865944255342404</v>
       </c>
-      <c r="K40" s="0" t="n">
+      <c r="L40" s="0" t="n">
+        <f aca="false">K40/B40</f>
+        <v>1.07905826210891E-006</v>
+      </c>
+      <c r="M40" s="0" t="n">
         <v>329.558744579851</v>
       </c>
-      <c r="L40" s="0" t="n">
-        <f aca="false">J40/B40</f>
-        <v>1.07905826210891E-006</v>
+      <c r="N40" s="1" t="n">
+        <f aca="false">SUM(G40:L40)</f>
+        <v>9.06218002994456</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>8267</v>
@@ -5533,28 +5873,36 @@
         <v>1548.30358531085</v>
       </c>
       <c r="G41" s="0" t="n">
+        <f aca="false">ABS(E41)</f>
+        <v>0.729755140053896</v>
+      </c>
+      <c r="H41" s="0" t="n">
         <v>0.187287236640964</v>
       </c>
-      <c r="H41" s="0" t="n">
+      <c r="I41" s="0" t="n">
         <v>7.16254466156471</v>
       </c>
-      <c r="I41" s="0" t="n">
+      <c r="J41" s="0" t="n">
         <v>0.000276782486151925</v>
       </c>
-      <c r="J41" s="0" t="n">
+      <c r="K41" s="0" t="n">
         <v>0.000806205405857607</v>
       </c>
-      <c r="K41" s="0" t="n">
+      <c r="L41" s="0" t="n">
+        <f aca="false">K41/B41</f>
+        <v>9.75209151878078E-008</v>
+      </c>
+      <c r="M41" s="0" t="n">
         <v>361.848998790195</v>
       </c>
-      <c r="L41" s="0" t="n">
-        <f aca="false">J41/B41</f>
-        <v>9.75209151878078E-008</v>
+      <c r="N41" s="1" t="n">
+        <f aca="false">SUM(G41:L41)</f>
+        <v>8.08067012367249</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>8557</v>
@@ -5572,28 +5920,36 @@
         <v>1578.87573019751</v>
       </c>
       <c r="G42" s="0" t="n">
+        <f aca="false">ABS(E42)</f>
+        <v>0.6752105575504</v>
+      </c>
+      <c r="H42" s="0" t="n">
         <v>0.184512765010811</v>
       </c>
-      <c r="H42" s="0" t="n">
+      <c r="I42" s="0" t="n">
         <v>4.54270822835517</v>
       </c>
-      <c r="I42" s="0" t="n">
+      <c r="J42" s="0" t="n">
         <v>0.000322668233027298</v>
       </c>
-      <c r="J42" s="0" t="n">
+      <c r="K42" s="0" t="n">
         <v>0.00131416241980807</v>
       </c>
-      <c r="K42" s="0" t="n">
+      <c r="L42" s="0" t="n">
+        <f aca="false">K42/B42</f>
+        <v>1.53577471053882E-007</v>
+      </c>
+      <c r="M42" s="0" t="n">
         <v>403.453190497187</v>
       </c>
-      <c r="L42" s="0" t="n">
-        <f aca="false">J42/B42</f>
-        <v>1.53577471053882E-007</v>
+      <c r="N42" s="1" t="n">
+        <f aca="false">SUM(G42:L42)</f>
+        <v>5.40406853514669</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>8710</v>
@@ -5611,28 +5967,36 @@
         <v>1692.66444640072</v>
       </c>
       <c r="G43" s="0" t="n">
+        <f aca="false">ABS(E43)</f>
+        <v>0.669449396748576</v>
+      </c>
+      <c r="H43" s="0" t="n">
         <v>0.194335757336477</v>
       </c>
-      <c r="H43" s="0" t="n">
+      <c r="I43" s="0" t="n">
         <v>4.45986451208441</v>
       </c>
-      <c r="I43" s="0" t="n">
+      <c r="J43" s="0" t="n">
         <v>0.000383716629183234</v>
       </c>
-      <c r="J43" s="0" t="n">
+      <c r="K43" s="0" t="n">
         <v>0.00314188655782225</v>
       </c>
-      <c r="K43" s="0" t="n">
+      <c r="L43" s="0" t="n">
+        <f aca="false">K43/B43</f>
+        <v>3.60721763240212E-007</v>
+      </c>
+      <c r="M43" s="0" t="n">
         <v>450.876913976468</v>
       </c>
-      <c r="L43" s="0" t="n">
-        <f aca="false">J43/B43</f>
-        <v>3.60721763240212E-007</v>
+      <c r="N43" s="1" t="n">
+        <f aca="false">SUM(G43:L43)</f>
+        <v>5.32717563007823</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>8853</v>
@@ -5650,28 +6014,36 @@
         <v>1692.8381009131</v>
       </c>
       <c r="G44" s="0" t="n">
+        <f aca="false">ABS(E44)</f>
+        <v>0.628466430922657</v>
+      </c>
+      <c r="H44" s="0" t="n">
         <v>0.191216322253823</v>
       </c>
-      <c r="H44" s="0" t="n">
+      <c r="I44" s="0" t="n">
         <v>5.192771197979</v>
       </c>
-      <c r="I44" s="0" t="n">
+      <c r="J44" s="0" t="n">
         <v>0.000491880318254834</v>
       </c>
-      <c r="J44" s="0" t="n">
+      <c r="K44" s="0" t="n">
         <v>0.00343144260914821</v>
       </c>
-      <c r="K44" s="0" t="n">
+      <c r="L44" s="0" t="n">
+        <f aca="false">K44/B44</f>
+        <v>3.87602237563336E-007</v>
+      </c>
+      <c r="M44" s="0" t="n">
         <v>499.187596301615</v>
       </c>
-      <c r="L44" s="0" t="n">
-        <f aca="false">J44/B44</f>
-        <v>3.87602237563336E-007</v>
+      <c r="N44" s="1" t="n">
+        <f aca="false">SUM(G44:L44)</f>
+        <v>6.01637766168512</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>8781</v>
@@ -5689,28 +6061,36 @@
         <v>1680.8216814692</v>
       </c>
       <c r="G45" s="0" t="n">
+        <f aca="false">ABS(E45)</f>
+        <v>0.631160678984458</v>
+      </c>
+      <c r="H45" s="0" t="n">
         <v>0.191415747804259</v>
       </c>
-      <c r="H45" s="0" t="n">
+      <c r="I45" s="0" t="n">
         <v>4.59462297617475</v>
       </c>
-      <c r="I45" s="0" t="n">
+      <c r="J45" s="0" t="n">
         <v>0.000580769246400757</v>
       </c>
-      <c r="J45" s="0" t="n">
+      <c r="K45" s="0" t="n">
         <v>0.00442369005090637</v>
       </c>
-      <c r="K45" s="0" t="n">
+      <c r="L45" s="0" t="n">
+        <f aca="false">K45/B45</f>
+        <v>5.03779757534036E-007</v>
+      </c>
+      <c r="M45" s="0" t="n">
         <v>595.988700198403</v>
       </c>
-      <c r="L45" s="0" t="n">
-        <f aca="false">J45/B45</f>
-        <v>5.03779757534036E-007</v>
+      <c r="N45" s="1" t="n">
+        <f aca="false">SUM(G45:L45)</f>
+        <v>5.42220436604053</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>8739</v>
@@ -5728,28 +6108,36 @@
         <v>1522.45695340046</v>
       </c>
       <c r="G46" s="0" t="n">
+        <f aca="false">ABS(E46)</f>
+        <v>0.654303596252078</v>
+      </c>
+      <c r="H46" s="0" t="n">
         <v>0.174214092390487</v>
       </c>
-      <c r="H46" s="0" t="n">
+      <c r="I46" s="0" t="n">
         <v>4.22970718748303</v>
       </c>
-      <c r="I46" s="0" t="n">
+      <c r="J46" s="0" t="n">
         <v>0.000626456336354074</v>
       </c>
-      <c r="J46" s="0" t="n">
+      <c r="K46" s="0" t="n">
         <v>0.00897830656593701</v>
       </c>
-      <c r="K46" s="0" t="n">
+      <c r="L46" s="0" t="n">
+        <f aca="false">K46/B46</f>
+        <v>1.02738374710345E-006</v>
+      </c>
+      <c r="M46" s="0" t="n">
         <v>630.97002109498</v>
       </c>
-      <c r="L46" s="0" t="n">
-        <f aca="false">J46/B46</f>
-        <v>1.02738374710345E-006</v>
+      <c r="N46" s="1" t="n">
+        <f aca="false">SUM(G46:L46)</f>
+        <v>5.06783066641163</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>8504</v>
@@ -5767,28 +6155,36 @@
         <v>1523.41838304642</v>
       </c>
       <c r="G47" s="0" t="n">
+        <f aca="false">ABS(E47)</f>
+        <v>0.645705010673964</v>
+      </c>
+      <c r="H47" s="0" t="n">
         <v>0.179141390292382</v>
       </c>
-      <c r="H47" s="0" t="n">
+      <c r="I47" s="0" t="n">
         <v>5.01504462915585</v>
       </c>
-      <c r="I47" s="0" t="n">
+      <c r="J47" s="0" t="n">
         <v>0.000564768509075626</v>
       </c>
-      <c r="J47" s="0" t="n">
+      <c r="K47" s="0" t="n">
         <v>0.0034142062709077</v>
       </c>
-      <c r="K47" s="0" t="n">
+      <c r="L47" s="0" t="n">
+        <f aca="false">K47/B47</f>
+        <v>4.01482393098271E-007</v>
+      </c>
+      <c r="M47" s="0" t="n">
         <v>656.043656990909</v>
       </c>
-      <c r="L47" s="0" t="n">
-        <f aca="false">J47/B47</f>
-        <v>4.01482393098271E-007</v>
+      <c r="N47" s="1" t="n">
+        <f aca="false">SUM(G47:L47)</f>
+        <v>5.84387040638457</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>7899</v>
@@ -5806,28 +6202,36 @@
         <v>1419.16223521432</v>
       </c>
       <c r="G48" s="0" t="n">
+        <f aca="false">ABS(E48)</f>
+        <v>0.37432428806207</v>
+      </c>
+      <c r="H48" s="0" t="n">
         <v>0.179663531486811</v>
       </c>
-      <c r="H48" s="0" t="n">
+      <c r="I48" s="0" t="n">
         <v>6.19812089007144</v>
       </c>
-      <c r="I48" s="0" t="n">
+      <c r="J48" s="0" t="n">
         <v>0.000610933715635278</v>
       </c>
-      <c r="J48" s="0" t="n">
+      <c r="K48" s="0" t="n">
         <v>0.00360067695934395</v>
       </c>
-      <c r="K48" s="0" t="n">
+      <c r="L48" s="0" t="n">
+        <f aca="false">K48/B48</f>
+        <v>4.55839594802374E-007</v>
+      </c>
+      <c r="M48" s="0" t="n">
         <v>678.164186826258</v>
       </c>
-      <c r="L48" s="0" t="n">
-        <f aca="false">J48/B48</f>
-        <v>4.55839594802374E-007</v>
+      <c r="N48" s="1" t="n">
+        <f aca="false">SUM(G48:L48)</f>
+        <v>6.7563207761349</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>8018</v>
@@ -5845,28 +6249,36 @@
         <v>1397.69287360925</v>
       </c>
       <c r="G49" s="0" t="n">
+        <f aca="false">ABS(E49)</f>
+        <v>0.395132313633951</v>
+      </c>
+      <c r="H49" s="0" t="n">
         <v>0.174319390572369</v>
       </c>
-      <c r="H49" s="0" t="n">
+      <c r="I49" s="0" t="n">
         <v>5.38771696486455</v>
       </c>
-      <c r="I49" s="0" t="n">
+      <c r="J49" s="0" t="n">
         <v>0.000636286874533817</v>
       </c>
-      <c r="J49" s="0" t="n">
+      <c r="K49" s="0" t="n">
         <v>0.00535801539572481</v>
       </c>
-      <c r="K49" s="0" t="n">
+      <c r="L49" s="0" t="n">
+        <f aca="false">K49/B49</f>
+        <v>6.68248365642905E-007</v>
+      </c>
+      <c r="M49" s="0" t="n">
         <v>680.940468290473</v>
       </c>
-      <c r="L49" s="0" t="n">
-        <f aca="false">J49/B49</f>
-        <v>6.68248365642905E-007</v>
+      <c r="N49" s="1" t="n">
+        <f aca="false">SUM(G49:L49)</f>
+        <v>5.9631636395895</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>8069</v>
@@ -5884,28 +6296,36 @@
         <v>1419.40804286901</v>
       </c>
       <c r="G50" s="0" t="n">
+        <f aca="false">ABS(E50)</f>
+        <v>0.363649850401885</v>
+      </c>
+      <c r="H50" s="0" t="n">
         <v>0.175908792027389</v>
       </c>
-      <c r="H50" s="0" t="n">
+      <c r="I50" s="0" t="n">
         <v>6.59339699851535</v>
       </c>
-      <c r="I50" s="0" t="n">
+      <c r="J50" s="0" t="n">
         <v>0.000676738171684243</v>
       </c>
-      <c r="J50" s="0" t="n">
+      <c r="K50" s="0" t="n">
         <v>0.00674356014113433</v>
       </c>
-      <c r="K50" s="0" t="n">
+      <c r="L50" s="0" t="n">
+        <f aca="false">K50/B50</f>
+        <v>8.35736787846614E-007</v>
+      </c>
+      <c r="M50" s="0" t="n">
         <v>699.067946539061</v>
       </c>
-      <c r="L50" s="0" t="n">
-        <f aca="false">J50/B50</f>
-        <v>8.35736787846614E-007</v>
+      <c r="N50" s="1" t="n">
+        <f aca="false">SUM(G50:L50)</f>
+        <v>7.14037677499423</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>8289</v>
@@ -5923,28 +6343,36 @@
         <v>1492.95713397538</v>
       </c>
       <c r="G51" s="0" t="n">
+        <f aca="false">ABS(E51)</f>
+        <v>0.35728993645904</v>
+      </c>
+      <c r="H51" s="0" t="n">
         <v>0.180113057543175</v>
       </c>
-      <c r="H51" s="0" t="n">
+      <c r="I51" s="0" t="n">
         <v>4.84161699024341</v>
       </c>
-      <c r="I51" s="0" t="n">
+      <c r="J51" s="0" t="n">
         <v>0.000697497622040771</v>
       </c>
-      <c r="J51" s="0" t="n">
+      <c r="K51" s="0" t="n">
         <v>0.00575429092217152</v>
       </c>
-      <c r="K51" s="0" t="n">
+      <c r="L51" s="0" t="n">
+        <f aca="false">K51/B51</f>
+        <v>6.94208097740562E-007</v>
+      </c>
+      <c r="M51" s="0" t="n">
         <v>717.965380590367</v>
       </c>
-      <c r="L51" s="0" t="n">
-        <f aca="false">J51/B51</f>
-        <v>6.94208097740562E-007</v>
+      <c r="N51" s="1" t="n">
+        <f aca="false">SUM(G51:L51)</f>
+        <v>5.38547246699794</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>8454</v>
@@ -5962,28 +6390,36 @@
         <v>1452.20260677079</v>
       </c>
       <c r="G52" s="0" t="n">
+        <f aca="false">ABS(E52)</f>
+        <v>0.408053255959629</v>
+      </c>
+      <c r="H52" s="0" t="n">
         <v>0.17177698211152</v>
       </c>
-      <c r="H52" s="0" t="n">
+      <c r="I52" s="0" t="n">
         <v>6.02608799450903</v>
       </c>
-      <c r="I52" s="0" t="n">
+      <c r="J52" s="0" t="n">
         <v>0.000617827983037266</v>
       </c>
-      <c r="J52" s="0" t="n">
+      <c r="K52" s="0" t="n">
         <v>0.00502904658579769</v>
       </c>
-      <c r="K52" s="0" t="n">
+      <c r="L52" s="0" t="n">
+        <f aca="false">K52/B52</f>
+        <v>5.94871845966133E-007</v>
+      </c>
+      <c r="M52" s="0" t="n">
         <v>736.930966986826</v>
       </c>
-      <c r="L52" s="0" t="n">
-        <f aca="false">J52/B52</f>
-        <v>5.94871845966133E-007</v>
+      <c r="N52" s="1" t="n">
+        <f aca="false">SUM(G52:L52)</f>
+        <v>6.61156570202086</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>8524</v>
@@ -6001,28 +6437,36 @@
         <v>1436.14324809036</v>
       </c>
       <c r="G53" s="0" t="n">
+        <f aca="false">ABS(E53)</f>
+        <v>0.414783229458891</v>
+      </c>
+      <c r="H53" s="0" t="n">
         <v>0.168482314416982</v>
       </c>
-      <c r="H53" s="0" t="n">
+      <c r="I53" s="0" t="n">
         <v>5.84852856839382</v>
       </c>
-      <c r="I53" s="0" t="n">
+      <c r="J53" s="0" t="n">
         <v>0.000728610444163581</v>
       </c>
-      <c r="J53" s="0" t="n">
+      <c r="K53" s="0" t="n">
         <v>0.00740435853254946</v>
       </c>
-      <c r="K53" s="0" t="n">
+      <c r="L53" s="0" t="n">
+        <f aca="false">K53/B53</f>
+        <v>8.68648349665587E-007</v>
+      </c>
+      <c r="M53" s="0" t="n">
         <v>741.561155526141</v>
       </c>
-      <c r="L53" s="0" t="n">
-        <f aca="false">J53/B53</f>
-        <v>8.68648349665587E-007</v>
+      <c r="N53" s="1" t="n">
+        <f aca="false">SUM(G53:L53)</f>
+        <v>6.43992794989476</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>8682</v>
@@ -6040,28 +6484,36 @@
         <v>1514.55662215757</v>
       </c>
       <c r="G54" s="0" t="n">
+        <f aca="false">ABS(E54)</f>
+        <v>0.345768193554335</v>
+      </c>
+      <c r="H54" s="0" t="n">
         <v>0.174447894742866</v>
       </c>
-      <c r="H54" s="0" t="n">
+      <c r="I54" s="0" t="n">
         <v>4.77751966603384</v>
       </c>
-      <c r="I54" s="0" t="n">
+      <c r="J54" s="0" t="n">
         <v>0.000603729512802379</v>
       </c>
-      <c r="J54" s="0" t="n">
+      <c r="K54" s="0" t="n">
         <v>0.00573535699114222</v>
       </c>
-      <c r="K54" s="0" t="n">
+      <c r="L54" s="0" t="n">
+        <f aca="false">K54/B54</f>
+        <v>6.60603201006936E-007</v>
+      </c>
+      <c r="M54" s="0" t="n">
         <v>758.400131105185</v>
       </c>
-      <c r="L54" s="0" t="n">
-        <f aca="false">J54/B54</f>
-        <v>6.60603201006936E-007</v>
+      <c r="N54" s="1" t="n">
+        <f aca="false">SUM(G54:L54)</f>
+        <v>5.30407550143819</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>8781</v>
@@ -6079,28 +6531,36 @@
         <v>1491.77196305213</v>
       </c>
       <c r="G55" s="0" t="n">
+        <f aca="false">ABS(E55)</f>
+        <v>0.370294377082132</v>
+      </c>
+      <c r="H55" s="0" t="n">
         <v>0.169886341311027</v>
       </c>
-      <c r="H55" s="0" t="n">
+      <c r="I55" s="0" t="n">
         <v>4.22122660549633</v>
       </c>
-      <c r="I55" s="0" t="n">
+      <c r="J55" s="0" t="n">
         <v>0.000644160359214054</v>
       </c>
-      <c r="J55" s="0" t="n">
+      <c r="K55" s="0" t="n">
         <v>0.00414892549887389</v>
       </c>
-      <c r="K55" s="0" t="n">
+      <c r="L55" s="0" t="n">
+        <f aca="false">K55/B55</f>
+        <v>4.72488953293918E-007</v>
+      </c>
+      <c r="M55" s="0" t="n">
         <v>762.644604057758</v>
       </c>
-      <c r="L55" s="0" t="n">
-        <f aca="false">J55/B55</f>
-        <v>4.72488953293918E-007</v>
+      <c r="N55" s="1" t="n">
+        <f aca="false">SUM(G55:L55)</f>
+        <v>4.76620088223653</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>8953</v>
@@ -6118,28 +6578,36 @@
         <v>1530.71193364544</v>
       </c>
       <c r="G56" s="0" t="n">
+        <f aca="false">ABS(E56)</f>
+        <v>0.419554206640157</v>
+      </c>
+      <c r="H56" s="0" t="n">
         <v>0.170971957293135</v>
       </c>
-      <c r="H56" s="0" t="n">
+      <c r="I56" s="0" t="n">
         <v>4.7229726743162</v>
       </c>
-      <c r="I56" s="0" t="n">
+      <c r="J56" s="0" t="n">
         <v>0.000609848397293071</v>
       </c>
-      <c r="J56" s="0" t="n">
+      <c r="K56" s="0" t="n">
         <v>0.0044734149299438</v>
       </c>
-      <c r="K56" s="0" t="n">
+      <c r="L56" s="0" t="n">
+        <f aca="false">K56/B56</f>
+        <v>4.99655414938434E-007</v>
+      </c>
+      <c r="M56" s="0" t="n">
         <v>781.9999117313</v>
       </c>
-      <c r="L56" s="0" t="n">
-        <f aca="false">J56/B56</f>
-        <v>4.99655414938434E-007</v>
+      <c r="N56" s="1" t="n">
+        <f aca="false">SUM(G56:L56)</f>
+        <v>5.31858260123214</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>8919</v>
@@ -6157,28 +6625,36 @@
         <v>1502.04007632069</v>
       </c>
       <c r="G57" s="0" t="n">
+        <f aca="false">ABS(E57)</f>
+        <v>0.337301003394742</v>
+      </c>
+      <c r="H57" s="0" t="n">
         <v>0.168409023020595</v>
       </c>
-      <c r="H57" s="0" t="n">
+      <c r="I57" s="0" t="n">
         <v>3.91142611171199</v>
       </c>
-      <c r="I57" s="0" t="n">
+      <c r="J57" s="0" t="n">
         <v>0.000683909359754138</v>
       </c>
-      <c r="J57" s="0" t="n">
+      <c r="K57" s="0" t="n">
         <v>0.00408486569958246</v>
       </c>
-      <c r="K57" s="0" t="n">
+      <c r="L57" s="0" t="n">
+        <f aca="false">K57/B57</f>
+        <v>4.57995929990185E-007</v>
+      </c>
+      <c r="M57" s="0" t="n">
         <v>785.419705175335</v>
       </c>
-      <c r="L57" s="0" t="n">
-        <f aca="false">J57/B57</f>
-        <v>4.57995929990185E-007</v>
+      <c r="N57" s="1" t="n">
+        <f aca="false">SUM(G57:L57)</f>
+        <v>4.42190537118259</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>9200</v>
@@ -6196,28 +6672,36 @@
         <v>1553.19319754817</v>
       </c>
       <c r="G58" s="0" t="n">
+        <f aca="false">ABS(E58)</f>
+        <v>0.36731237771491</v>
+      </c>
+      <c r="H58" s="0" t="n">
         <v>0.168825347559584</v>
       </c>
-      <c r="H58" s="0" t="n">
+      <c r="I58" s="0" t="n">
         <v>5.22357592455819</v>
       </c>
-      <c r="I58" s="0" t="n">
+      <c r="J58" s="0" t="n">
         <v>0.00078054516736937</v>
       </c>
-      <c r="J58" s="0" t="n">
+      <c r="K58" s="0" t="n">
         <v>0.00766257737779833</v>
       </c>
-      <c r="K58" s="0" t="n">
+      <c r="L58" s="0" t="n">
+        <f aca="false">K58/B58</f>
+        <v>8.32888845412862E-007</v>
+      </c>
+      <c r="M58" s="0" t="n">
         <v>804.093801721934</v>
       </c>
-      <c r="L58" s="0" t="n">
-        <f aca="false">J58/B58</f>
-        <v>8.32888845412862E-007</v>
+      <c r="N58" s="1" t="n">
+        <f aca="false">SUM(G58:L58)</f>
+        <v>5.7681576052667</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>9191</v>
@@ -6235,24 +6719,36 @@
         <v>1562.65138868961</v>
       </c>
       <c r="G59" s="0" t="n">
+        <f aca="false">ABS(E59)</f>
+        <v>0.262240712524942</v>
+      </c>
+      <c r="H59" s="0" t="n">
         <v>0.170019735468351</v>
       </c>
-      <c r="H59" s="0" t="n">
+      <c r="I59" s="0" t="n">
         <v>5.21054777416958</v>
       </c>
-      <c r="I59" s="0" t="n">
+      <c r="J59" s="0" t="n">
         <v>0.000925816944321923</v>
       </c>
-      <c r="J59" s="0" t="n">
+      <c r="K59" s="0" t="n">
         <v>0.0166148617904466</v>
       </c>
-      <c r="K59" s="0" t="n">
+      <c r="L59" s="0" t="n">
+        <f aca="false">K59/B59</f>
+        <v>1.80773167124868E-006</v>
+      </c>
+      <c r="M59" s="0" t="n">
         <v>809.357784286451</v>
+      </c>
+      <c r="N59" s="1" t="n">
+        <f aca="false">SUM(G59:L59)</f>
+        <v>5.66035070862931</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>9434</v>
@@ -6270,28 +6766,36 @@
         <v>1499.41512539275</v>
       </c>
       <c r="G60" s="0" t="n">
+        <f aca="false">ABS(E60)</f>
+        <v>0.360696797384634</v>
+      </c>
+      <c r="H60" s="0" t="n">
         <v>0.158937367542161</v>
       </c>
-      <c r="H60" s="0" t="n">
+      <c r="I60" s="0" t="n">
         <v>4.24847984430977</v>
       </c>
-      <c r="I60" s="0" t="n">
+      <c r="J60" s="0" t="n">
         <v>0.000768293599203474</v>
       </c>
-      <c r="J60" s="0" t="n">
+      <c r="K60" s="0" t="n">
         <v>0.00663771067877741</v>
       </c>
-      <c r="K60" s="0" t="n">
+      <c r="L60" s="0" t="n">
+        <f aca="false">K60/B60</f>
+        <v>7.03594517572335E-007</v>
+      </c>
+      <c r="M60" s="0" t="n">
         <v>824.548795750479</v>
       </c>
-      <c r="L60" s="0" t="n">
-        <f aca="false">J60/B60</f>
-        <v>7.03594517572335E-007</v>
+      <c r="N60" s="1" t="n">
+        <f aca="false">SUM(G60:L60)</f>
+        <v>4.77552071710906</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>9360</v>
@@ -6309,28 +6813,36 @@
         <v>1625.24018565245</v>
       </c>
       <c r="G61" s="0" t="n">
+        <f aca="false">ABS(E61)</f>
+        <v>0.267452923691422</v>
+      </c>
+      <c r="H61" s="0" t="n">
         <v>0.173636771971415</v>
       </c>
-      <c r="H61" s="0" t="n">
+      <c r="I61" s="0" t="n">
         <v>4.34949475832994</v>
       </c>
-      <c r="I61" s="0" t="n">
+      <c r="J61" s="0" t="n">
         <v>0.000825015063042073</v>
       </c>
-      <c r="J61" s="0" t="n">
+      <c r="K61" s="0" t="n">
         <v>0.00664414106427944</v>
       </c>
-      <c r="K61" s="0" t="n">
+      <c r="L61" s="0" t="n">
+        <f aca="false">K61/B61</f>
+        <v>7.09844130799086E-007</v>
+      </c>
+      <c r="M61" s="0" t="n">
         <v>825.256143537636</v>
       </c>
-      <c r="L61" s="0" t="n">
-        <f aca="false">J61/B61</f>
-        <v>7.09844130799086E-007</v>
+      <c r="N61" s="1" t="n">
+        <f aca="false">SUM(G61:L61)</f>
+        <v>4.79805431996423</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>9447</v>
@@ -6348,28 +6860,36 @@
         <v>1541.53573584119</v>
       </c>
       <c r="G62" s="0" t="n">
+        <f aca="false">ABS(E62)</f>
+        <v>0.319391086719577</v>
+      </c>
+      <c r="H62" s="0" t="n">
         <v>0.163177277002349</v>
       </c>
-      <c r="H62" s="0" t="n">
+      <c r="I62" s="0" t="n">
         <v>3.5970355526143</v>
       </c>
-      <c r="I62" s="0" t="n">
+      <c r="J62" s="0" t="n">
         <v>0.000809246850196785</v>
       </c>
-      <c r="J62" s="0" t="n">
+      <c r="K62" s="0" t="n">
         <v>0.00655855690743985</v>
       </c>
-      <c r="K62" s="0" t="n">
+      <c r="L62" s="0" t="n">
+        <f aca="false">K62/B62</f>
+        <v>6.94247582030258E-007</v>
+      </c>
+      <c r="M62" s="0" t="n">
         <v>834.92656881569</v>
       </c>
-      <c r="L62" s="0" t="n">
-        <f aca="false">J62/B62</f>
-        <v>6.94247582030258E-007</v>
+      <c r="N62" s="1" t="n">
+        <f aca="false">SUM(G62:L62)</f>
+        <v>4.08697241434145</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>9580</v>
@@ -6387,28 +6907,36 @@
         <v>1582.94257168919</v>
       </c>
       <c r="G63" s="0" t="n">
+        <f aca="false">ABS(E63)</f>
+        <v>0.342008328290831</v>
+      </c>
+      <c r="H63" s="0" t="n">
         <v>0.165234088902838</v>
       </c>
-      <c r="H63" s="0" t="n">
+      <c r="I63" s="0" t="n">
         <v>4.43853874806436</v>
       </c>
-      <c r="I63" s="0" t="n">
+      <c r="J63" s="0" t="n">
         <v>0.00084883789384596</v>
       </c>
-      <c r="J63" s="0" t="n">
+      <c r="K63" s="0" t="n">
         <v>0.00885730504113845</v>
       </c>
-      <c r="K63" s="0" t="n">
+      <c r="L63" s="0" t="n">
+        <f aca="false">K63/B63</f>
+        <v>9.24562112853701E-007</v>
+      </c>
+      <c r="M63" s="0" t="n">
         <v>837.801547813215</v>
       </c>
-      <c r="L63" s="0" t="n">
-        <f aca="false">J63/B63</f>
-        <v>9.24562112853701E-007</v>
+      <c r="N63" s="1" t="n">
+        <f aca="false">SUM(G63:L63)</f>
+        <v>4.95548823275513</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>9470</v>
@@ -6426,28 +6954,36 @@
         <v>1433.0517847562</v>
       </c>
       <c r="G64" s="0" t="n">
+        <f aca="false">ABS(E64)</f>
+        <v>0.314284228823936</v>
+      </c>
+      <c r="H64" s="0" t="n">
         <v>0.151325426056621</v>
       </c>
-      <c r="H64" s="0" t="n">
+      <c r="I64" s="0" t="n">
         <v>3.99608719542223</v>
       </c>
-      <c r="I64" s="0" t="n">
+      <c r="J64" s="0" t="n">
         <v>0.000779821692007022</v>
       </c>
-      <c r="J64" s="0" t="n">
+      <c r="K64" s="0" t="n">
         <v>0.00554621264038529</v>
       </c>
-      <c r="K64" s="0" t="n">
+      <c r="L64" s="0" t="n">
+        <f aca="false">K64/B64</f>
+        <v>5.85661313662649E-007</v>
+      </c>
+      <c r="M64" s="0" t="n">
         <v>838.899276955448</v>
       </c>
-      <c r="L64" s="0" t="n">
-        <f aca="false">J64/B64</f>
-        <v>5.85661313662649E-007</v>
+      <c r="N64" s="1" t="n">
+        <f aca="false">SUM(G64:L64)</f>
+        <v>4.46802347029649</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>9513</v>
@@ -6465,28 +7001,36 @@
         <v>1617.96575008942</v>
       </c>
       <c r="G65" s="0" t="n">
+        <f aca="false">ABS(E65)</f>
+        <v>0.292256687521643</v>
+      </c>
+      <c r="H65" s="0" t="n">
         <v>0.170079443928248</v>
       </c>
-      <c r="H65" s="0" t="n">
+      <c r="I65" s="0" t="n">
         <v>4.28225602939202</v>
       </c>
-      <c r="I65" s="0" t="n">
+      <c r="J65" s="0" t="n">
         <v>0.000992019575501817</v>
       </c>
-      <c r="J65" s="0" t="n">
+      <c r="K65" s="0" t="n">
         <v>0.0093486838559575</v>
       </c>
-      <c r="K65" s="0" t="n">
+      <c r="L65" s="0" t="n">
+        <f aca="false">K65/B65</f>
+        <v>9.82727200247819E-007</v>
+      </c>
+      <c r="M65" s="0" t="n">
         <v>843.423958654543</v>
       </c>
-      <c r="L65" s="0" t="n">
-        <f aca="false">J65/B65</f>
-        <v>9.82727200247819E-007</v>
+      <c r="N65" s="1" t="n">
+        <f aca="false">SUM(G65:L65)</f>
+        <v>4.75493384700057</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>9590</v>
@@ -6504,28 +7048,36 @@
         <v>1604.2672539986</v>
       </c>
       <c r="G66" s="0" t="n">
+        <f aca="false">ABS(E66)</f>
+        <v>0.292785545938358</v>
+      </c>
+      <c r="H66" s="0" t="n">
         <v>0.167285427945631</v>
       </c>
-      <c r="H66" s="0" t="n">
+      <c r="I66" s="0" t="n">
         <v>4.637996555016</v>
       </c>
-      <c r="I66" s="0" t="n">
+      <c r="J66" s="0" t="n">
         <v>0.00104489312826321</v>
       </c>
-      <c r="J66" s="0" t="n">
+      <c r="K66" s="0" t="n">
         <v>0.0133460518601946</v>
       </c>
-      <c r="K66" s="0" t="n">
+      <c r="L66" s="0" t="n">
+        <f aca="false">K66/B66</f>
+        <v>1.3916633847961E-006</v>
+      </c>
+      <c r="M66" s="0" t="n">
         <v>845.123879794779</v>
       </c>
-      <c r="L66" s="0" t="n">
-        <f aca="false">J66/B66</f>
-        <v>1.3916633847961E-006</v>
+      <c r="N66" s="1" t="n">
+        <f aca="false">SUM(G66:L66)</f>
+        <v>5.11245986555183</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>9537</v>
@@ -6543,27 +7095,33 @@
         <v>1495.62959310693</v>
       </c>
       <c r="G67" s="0" t="n">
+        <f aca="false">ABS(E67)</f>
+        <v>0.280080366172712</v>
+      </c>
+      <c r="H67" s="0" t="n">
         <v>0.156823906166187</v>
       </c>
-      <c r="H67" s="0" t="n">
+      <c r="I67" s="0" t="n">
         <v>4.58644437945878</v>
       </c>
-      <c r="I67" s="0" t="n">
+      <c r="J67" s="0" t="n">
         <v>0.000828118827530218</v>
       </c>
-      <c r="J67" s="0" t="n">
+      <c r="K67" s="0" t="n">
         <v>0.00659421582941922</v>
       </c>
-      <c r="K67" s="0" t="n">
+      <c r="L67" s="0" t="n">
+        <f aca="false">K67/B67</f>
+        <v>6.91435024579975E-007</v>
+      </c>
+      <c r="M67" s="0" t="n">
         <v>846.008194632081</v>
       </c>
-      <c r="L67" s="0" t="n">
-        <f aca="false">J67/B67</f>
-        <v>6.91435024579975E-007</v>
+      <c r="N67" s="1" t="n">
+        <f aca="false">SUM(G67:L67)</f>
+        <v>5.03077167788965</v>
       </c>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <conditionalFormatting sqref="D2:D67">
     <cfRule type="colorScale" priority="2">
@@ -6577,7 +7135,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F67">
+  <conditionalFormatting sqref="H2:H67">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="percentile" val="10"/>
@@ -6589,7 +7147,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G67">
+  <conditionalFormatting sqref="I2:I67">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="percentile" val="10"/>
@@ -6601,7 +7159,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H67">
+  <conditionalFormatting sqref="J2:J67">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="percentile" val="10"/>
@@ -6613,19 +7171,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I67">
+  <conditionalFormatting sqref="K2:K67">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="percentile" val="10"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="percentile" val="90"/>
-        <color rgb="FF00FF00"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF00CC00"/>
         <color rgb="FFFFFF00"/>
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J67">
+  <conditionalFormatting sqref="L2:L67">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -6637,13 +7195,37 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L67">
+  <conditionalFormatting sqref="G2:G67">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max" val="0"/>
         <color rgb="FF00CC00"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N1:N67">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF00CC00"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F67">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="percentile" val="10"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="90"/>
+        <color rgb="FF00FF00"/>
         <color rgb="FFFFFF00"/>
         <color rgb="FFFF0000"/>
       </colorScale>

</xml_diff>